<commit_message>
cleanup before commands branch
</commit_message>
<xml_diff>
--- a/H89_ESP32 Commands.xlsx
+++ b/H89_ESP32 Commands.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dev\ESP32\H89_ESP32\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dev\ESP32\H89_ESP32\Nice Try\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CEF28F4-B46F-4E0E-9CE3-5F25162E3DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD2C69B-E1F6-491F-8F91-FB4EC5BA664B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4635" yWindow="1980" windowWidth="22530" windowHeight="12615" activeTab="6" xr2:uid="{D2F2CCC8-256C-4E0F-AF5D-63EDFF332B66}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="22530" windowHeight="12615" activeTab="6" xr2:uid="{D2F2CCC8-256C-4E0F-AF5D-63EDFF332B66}"/>
   </bookViews>
   <sheets>
     <sheet name="Commands" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="ESP32 Pins" sheetId="6" r:id="rId8"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">'Cmd Summary'!$A$1:$G$12</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Commands!$A$1:$U$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="227">
   <si>
     <t>Read Port Function</t>
   </si>
@@ -637,9 +638,6 @@
     <t>Read # sectors, update disk image</t>
   </si>
   <si>
-    <t>Update last operation status</t>
-  </si>
-  <si>
     <t>Zero terminated string with list of files on SD card</t>
   </si>
   <si>
@@ -652,15 +650,9 @@
     <t>0A</t>
   </si>
   <si>
-    <t>0B</t>
-  </si>
-  <si>
     <t>2A</t>
   </si>
   <si>
-    <t>2B</t>
-  </si>
-  <si>
     <t>Varies</t>
   </si>
   <si>
@@ -728,6 +720,12 @@
   </si>
   <si>
     <t>Disk 3 bits + LBA MSB 5 bits</t>
+  </si>
+  <si>
+    <t>Debug</t>
+  </si>
+  <si>
+    <t>Return same four bytes + offset. Offset increases by one each time command is sent.</t>
   </si>
 </sst>
 </file>
@@ -840,7 +838,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -1037,12 +1035,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1219,23 +1230,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1255,6 +1251,49 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1758,16 +1797,16 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="F6" s="2"/>
-      <c r="G6" s="66">
+      <c r="G6" s="78">
         <v>1</v>
       </c>
-      <c r="H6" s="67"/>
-      <c r="I6" s="67"/>
-      <c r="J6" s="66">
+      <c r="H6" s="79"/>
+      <c r="I6" s="79"/>
+      <c r="J6" s="78">
         <v>0</v>
       </c>
-      <c r="K6" s="67"/>
-      <c r="L6" s="67"/>
+      <c r="K6" s="79"/>
+      <c r="L6" s="79"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="X6" s="2" t="s">
@@ -1778,16 +1817,16 @@
       <c r="F7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="68" t="s">
+      <c r="G7" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="69"/>
-      <c r="I7" s="69"/>
-      <c r="J7" s="68" t="s">
+      <c r="H7" s="77"/>
+      <c r="I7" s="77"/>
+      <c r="J7" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="K7" s="69"/>
-      <c r="L7" s="69"/>
+      <c r="K7" s="77"/>
+      <c r="L7" s="77"/>
       <c r="X7" s="1" t="s">
         <v>68</v>
       </c>
@@ -1802,21 +1841,21 @@
       <c r="F8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="68" t="s">
+      <c r="G8" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="69"/>
-      <c r="I8" s="69"/>
-      <c r="J8" s="68" t="s">
+      <c r="H8" s="77"/>
+      <c r="I8" s="77"/>
+      <c r="J8" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="K8" s="69"/>
-      <c r="L8" s="69"/>
+      <c r="K8" s="77"/>
+      <c r="L8" s="77"/>
       <c r="O8" s="17"/>
-      <c r="P8" s="70" t="s">
+      <c r="P8" s="74" t="s">
         <v>61</v>
       </c>
-      <c r="Q8" s="71"/>
+      <c r="Q8" s="75"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
       <c r="Y8" s="1" t="s">
@@ -1830,16 +1869,16 @@
       <c r="F9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="68" t="s">
+      <c r="G9" s="76" t="s">
         <v>58</v>
       </c>
-      <c r="H9" s="69"/>
-      <c r="I9" s="69"/>
-      <c r="J9" s="68" t="s">
+      <c r="H9" s="77"/>
+      <c r="I9" s="77"/>
+      <c r="J9" s="76" t="s">
         <v>59</v>
       </c>
-      <c r="K9" s="69"/>
-      <c r="L9" s="69"/>
+      <c r="K9" s="77"/>
+      <c r="L9" s="77"/>
       <c r="O9" s="58" t="s">
         <v>66</v>
       </c>
@@ -1867,16 +1906,16 @@
       <c r="F10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="68" t="s">
+      <c r="G10" s="76" t="s">
         <v>83</v>
       </c>
-      <c r="H10" s="69"/>
-      <c r="I10" s="69"/>
-      <c r="J10" s="68" t="s">
+      <c r="H10" s="77"/>
+      <c r="I10" s="77"/>
+      <c r="J10" s="76" t="s">
         <v>84</v>
       </c>
-      <c r="K10" s="69"/>
-      <c r="L10" s="69"/>
+      <c r="K10" s="77"/>
+      <c r="L10" s="77"/>
       <c r="O10" s="42" t="s">
         <v>62</v>
       </c>
@@ -2375,17 +2414,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="J8:L8"/>
     <mergeCell ref="P8:Q8"/>
     <mergeCell ref="J9:L9"/>
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="G9:I9"/>
     <mergeCell ref="G10:I10"/>
     <mergeCell ref="J10:L10"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="J8:L8"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3949,15 +3988,18 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA02D72B-19E2-4159-802E-21717FF6578A}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="77" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" style="72" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" customWidth="1"/>
     <col min="6" max="6" width="12.140625" customWidth="1"/>
@@ -3971,7 +4013,7 @@
         <v>43</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C1" s="60" t="s">
         <v>193</v>
@@ -3988,7 +4030,9 @@
       <c r="G1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="H1" s="2"/>
+      <c r="H1" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -4021,13 +4065,13 @@
         <v>4</v>
       </c>
       <c r="D3" s="62" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E3" s="62" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="F3" s="62" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G3" s="63" t="s">
         <v>186</v>
@@ -4040,19 +4084,19 @@
         <v>175</v>
       </c>
       <c r="B4" s="64" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C4" s="64">
         <v>4</v>
       </c>
       <c r="D4" s="62" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E4" s="62" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="F4" s="62" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G4" s="63" t="s">
         <v>196</v>
@@ -4073,48 +4117,44 @@
         <v>8388608</v>
       </c>
       <c r="O4" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="63" t="s">
-        <v>185</v>
-      </c>
-      <c r="B5" s="64" t="s">
-        <v>202</v>
-      </c>
-      <c r="C5" s="64">
-        <v>3</v>
-      </c>
-      <c r="D5" s="62" t="s">
-        <v>212</v>
-      </c>
-      <c r="E5" s="62" t="s">
-        <v>213</v>
-      </c>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="67"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
       <c r="F5" s="62"/>
-      <c r="G5" s="63" t="s">
-        <v>197</v>
-      </c>
-      <c r="H5" s="61"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="66"/>
       <c r="I5" s="1"/>
       <c r="N5">
         <f>L4*M4</f>
         <v>8192</v>
       </c>
       <c r="O5" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="63"/>
-      <c r="B6" s="64"/>
-      <c r="C6" s="64"/>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="67" t="s">
+        <v>180</v>
+      </c>
+      <c r="B6" s="64">
+        <v>10</v>
+      </c>
+      <c r="C6" s="64">
+        <v>1</v>
+      </c>
       <c r="D6" s="62"/>
       <c r="E6" s="62"/>
       <c r="F6" s="62"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="61"/>
+      <c r="G6" s="67" t="s">
+        <v>197</v>
+      </c>
+      <c r="H6" s="66"/>
       <c r="I6" s="1"/>
       <c r="K6">
         <v>256</v>
@@ -4127,23 +4167,27 @@
         <v>65536</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="63" t="s">
-        <v>180</v>
+    <row r="7" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="67" t="s">
+        <v>181</v>
       </c>
       <c r="B7" s="64">
-        <v>10</v>
-      </c>
-      <c r="C7" s="64">
-        <v>1</v>
-      </c>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="63" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="64" t="s">
+        <v>202</v>
+      </c>
+      <c r="D7" s="62" t="s">
+        <v>221</v>
+      </c>
+      <c r="E7" s="67" t="s">
+        <v>203</v>
+      </c>
+      <c r="F7" s="67"/>
+      <c r="G7" s="73" t="s">
         <v>198</v>
       </c>
-      <c r="H7" s="61"/>
+      <c r="H7" s="66"/>
       <c r="I7" s="1"/>
       <c r="K7">
         <v>2</v>
@@ -4157,135 +4201,116 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="63" t="s">
+      <c r="A8" s="67" t="s">
         <v>181</v>
       </c>
       <c r="B8" s="64">
-        <v>11</v>
-      </c>
-      <c r="C8" s="64" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="64">
+        <v>3</v>
+      </c>
+      <c r="D8" s="62" t="s">
+        <v>221</v>
+      </c>
+      <c r="E8" s="68" t="s">
+        <v>204</v>
+      </c>
+      <c r="F8" s="69"/>
+      <c r="G8" s="73" t="s">
+        <v>198</v>
+      </c>
+      <c r="H8" s="66"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="67" t="s">
+        <v>174</v>
+      </c>
+      <c r="B9" s="64">
+        <v>28</v>
+      </c>
+      <c r="C9" s="64">
+        <v>4</v>
+      </c>
+      <c r="D9" s="62" t="s">
+        <v>223</v>
+      </c>
+      <c r="E9" s="62" t="s">
         <v>205</v>
       </c>
-      <c r="D8" s="62" t="s">
-        <v>224</v>
-      </c>
-      <c r="E8" s="72" t="s">
+      <c r="F9" s="62" t="s">
         <v>206</v>
       </c>
-      <c r="F8" s="72"/>
-      <c r="G8" s="78" t="s">
-        <v>199</v>
-      </c>
-      <c r="H8" s="61"/>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="63" t="s">
-        <v>181</v>
-      </c>
-      <c r="B9" s="64">
-        <v>12</v>
-      </c>
-      <c r="C9" s="64">
-        <v>3</v>
-      </c>
-      <c r="D9" s="62" t="s">
-        <v>224</v>
-      </c>
-      <c r="E9" s="73" t="s">
-        <v>207</v>
-      </c>
-      <c r="F9" s="74"/>
-      <c r="G9" s="78" t="s">
-        <v>199</v>
-      </c>
-      <c r="H9" s="61"/>
+      <c r="G9" s="67" t="s">
+        <v>186</v>
+      </c>
+      <c r="H9" s="67"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="63" t="s">
-        <v>174</v>
-      </c>
-      <c r="B10" s="64">
-        <v>28</v>
+    <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="67" t="s">
+        <v>175</v>
+      </c>
+      <c r="B10" s="64" t="s">
+        <v>201</v>
       </c>
       <c r="C10" s="64">
         <v>4</v>
       </c>
       <c r="D10" s="62" t="s">
+        <v>223</v>
+      </c>
+      <c r="E10" s="62" t="s">
+        <v>205</v>
+      </c>
+      <c r="F10" s="62" t="s">
+        <v>206</v>
+      </c>
+      <c r="G10" s="67" t="s">
+        <v>196</v>
+      </c>
+      <c r="H10" s="67"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="D11" s="80" t="s">
+        <v>224</v>
+      </c>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="81" t="s">
+        <v>225</v>
+      </c>
+      <c r="B12" s="88">
+        <v>1</v>
+      </c>
+      <c r="C12" s="83">
+        <v>4</v>
+      </c>
+      <c r="D12" s="84" t="s">
+        <v>184</v>
+      </c>
+      <c r="E12" s="85" t="s">
+        <v>184</v>
+      </c>
+      <c r="F12" s="82" t="s">
+        <v>184</v>
+      </c>
+      <c r="G12" s="86" t="s">
         <v>226</v>
       </c>
-      <c r="E10" s="62" t="s">
-        <v>208</v>
-      </c>
-      <c r="F10" s="62" t="s">
-        <v>209</v>
-      </c>
-      <c r="G10" s="63" t="s">
-        <v>186</v>
-      </c>
-      <c r="H10" s="63"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="63" t="s">
-        <v>175</v>
-      </c>
-      <c r="B11" s="64" t="s">
-        <v>203</v>
-      </c>
-      <c r="C11" s="64">
-        <v>4</v>
-      </c>
-      <c r="D11" s="62" t="s">
-        <v>226</v>
-      </c>
-      <c r="E11" s="62" t="s">
-        <v>208</v>
-      </c>
-      <c r="F11" s="62" t="s">
-        <v>209</v>
-      </c>
-      <c r="G11" s="63" t="s">
-        <v>196</v>
-      </c>
-      <c r="H11" s="63"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="63" t="s">
-        <v>185</v>
-      </c>
-      <c r="B12" s="64" t="s">
-        <v>204</v>
-      </c>
-      <c r="C12" s="64">
-        <v>3</v>
-      </c>
-      <c r="D12" s="62" t="s">
-        <v>226</v>
-      </c>
-      <c r="E12" s="62" t="s">
-        <v>208</v>
-      </c>
-      <c r="F12" s="62"/>
-      <c r="G12" s="63"/>
-      <c r="H12" s="63"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="D13" s="63" t="s">
-        <v>227</v>
-      </c>
+      <c r="H12" s="87"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C15" s="75" t="s">
-        <v>215</v>
+      <c r="C15" s="70" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -4295,14 +4320,14 @@
         <v>10000000</v>
       </c>
       <c r="G17" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>225</v>
-      </c>
-      <c r="D18" s="76">
+        <v>222</v>
+      </c>
+      <c r="D18" s="71">
         <f>N4</f>
         <v>8388608</v>
       </c>
@@ -4311,24 +4336,24 @@
         <v>#NUM!</v>
       </c>
       <c r="G18" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D19">
         <v>3</v>
       </c>
       <c r="E19" s="22"/>
       <c r="G19" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D20">
         <v>2</v>
@@ -4338,12 +4363,12 @@
         <v>10</v>
       </c>
       <c r="G20" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D21" s="22" t="e">
         <f>DEC2BIN(D17*64+D18/POWER(2,D19)+D20)</f>
@@ -4352,7 +4377,7 @@
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D22" s="65">
         <f>D17*64+D18/POWER(2,D19)+D20</f>
@@ -4360,13 +4385,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-  </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
File upload from H89 to ESP32 using xmodem Updated Data In Buffer Pointers to loop when reaching end of buffer. Buffer full Flag Added functions to print Buffer status, getDataTime gets data with timeout in ms
</commit_message>
<xml_diff>
--- a/H89_ESP32 Commands.xlsx
+++ b/H89_ESP32 Commands.xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dev\ESP32\H89_ESP32\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB370DE4-0F0F-4A28-B691-F4D9E57846BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5045C9-E77C-4648-B2B5-C607F2506F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31155" yWindow="2370" windowWidth="21600" windowHeight="11385" tabRatio="636" activeTab="1" xr2:uid="{D2F2CCC8-256C-4E0F-AF5D-63EDFF332B66}"/>
+    <workbookView xWindow="29730" yWindow="3330" windowWidth="21600" windowHeight="11385" tabRatio="636" activeTab="2" xr2:uid="{D2F2CCC8-256C-4E0F-AF5D-63EDFF332B66}"/>
   </bookViews>
   <sheets>
     <sheet name="Cmd Summary" sheetId="8" r:id="rId1"/>
     <sheet name="Code" sheetId="9" r:id="rId2"/>
-    <sheet name="ESP32 Pins" sheetId="6" r:id="rId3"/>
-    <sheet name="PCB Notes" sheetId="10" r:id="rId4"/>
-    <sheet name="Commands" sheetId="1" r:id="rId5"/>
-    <sheet name="Timing" sheetId="4" r:id="rId6"/>
-    <sheet name="Breadboard" sheetId="3" r:id="rId7"/>
-    <sheet name="LM317T" sheetId="2" r:id="rId8"/>
-    <sheet name="573 245 " sheetId="5" r:id="rId9"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId10"/>
+    <sheet name="Sheet2" sheetId="11" r:id="rId3"/>
+    <sheet name="ESP32 Pins" sheetId="6" r:id="rId4"/>
+    <sheet name="PCB Notes" sheetId="10" r:id="rId5"/>
+    <sheet name="Commands" sheetId="1" r:id="rId6"/>
+    <sheet name="Timing" sheetId="4" r:id="rId7"/>
+    <sheet name="Breadboard" sheetId="3" r:id="rId8"/>
+    <sheet name="LM317T" sheetId="2" r:id="rId9"/>
+    <sheet name="573 245 " sheetId="5" r:id="rId10"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Cmd Summary'!$A$1:$G$22</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">Commands!$A$1:$U$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">Commands!$A$1:$U$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="312">
   <si>
     <t>Read Port Function</t>
   </si>
@@ -1017,6 +1018,210 @@
       <t xml:space="preserve"> to ESP_BSY</t>
     </r>
   </si>
+  <si>
+    <t>Timing</t>
+  </si>
+  <si>
+    <t>Bytes</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>Period uS</t>
+  </si>
+  <si>
+    <t>Hz</t>
+  </si>
+  <si>
+    <t>Duration uS</t>
+  </si>
+  <si>
+    <t>Interrupt</t>
+  </si>
+  <si>
+    <t>// Command control bytes</t>
+  </si>
+  <si>
+    <t>// Data out bytes</t>
+  </si>
+  <si>
+    <t>extern int currentStatus  ;          // status value for H89 to read</t>
+  </si>
+  <si>
+    <t>extern int h89ReadData  ;    // status value for H89 data actually read</t>
+  </si>
+  <si>
+    <t>extern int h89BytesToRead ;</t>
+  </si>
+  <si>
+    <t>volatile int dataInPtr = 0;           // Ptr to next position to write data</t>
+  </si>
+  <si>
+    <t>volatile byte cmdData[CMD_LENGTH];    // command data buffer</t>
+  </si>
+  <si>
+    <t>volatile int8_t cmdFlag = 0;          // processing a command flag</t>
+  </si>
+  <si>
+    <t>volatile int8_t cmdLen = CMD_LENGTH;  // max length for a command</t>
+  </si>
+  <si>
+    <t>volatile int dataOutBufLast = 0;        // Last valid data in send buffer</t>
+  </si>
+  <si>
+    <t>setStatusPort(byte status)</t>
+  </si>
+  <si>
+    <t>Writes status to H89 Port</t>
+  </si>
+  <si>
+    <t>Writes statu in global currenStatus</t>
+  </si>
+  <si>
+    <t>  //************** H89 data flags</t>
+  </si>
+  <si>
+    <t>volatile int dataOutBufPtr = 0;         // Ptr to next byte to send to H89</t>
+  </si>
+  <si>
+    <t>volatile byte cmdDataPtr = 0 ;        // Ptr to last valid data, -1 means no valid data</t>
+  </si>
+  <si>
+    <t>volatile byte dataInBuf[BUFFER_LEN] ;        // data received from H89</t>
+  </si>
+  <si>
+    <t>volatile byte dataOutBuf[BUFFER_LEN];         // data to send to H89</t>
+  </si>
+  <si>
+    <t>volatile int dataInLast = 0;          // pointer to valid data. No data iof dataInLast = dataInPtr</t>
+  </si>
+  <si>
+    <t>volatile bool bufferFull = false;     // flag to indicate buffer is full</t>
+  </si>
+  <si>
+    <t>  //************** H89 data  In buffers</t>
+  </si>
+  <si>
+    <t>Status Port</t>
+  </si>
+  <si>
+    <t>CurrentStatus</t>
+  </si>
+  <si>
+    <t>CmdDataPtr</t>
+  </si>
+  <si>
+    <t>CmdFlag</t>
+  </si>
+  <si>
+    <t>H89BytesToRead</t>
+  </si>
+  <si>
+    <t>h89ReadData</t>
+  </si>
+  <si>
+    <t>H89_WRITE_OK</t>
+  </si>
+  <si>
+    <t>ESP_BUSY</t>
+  </si>
+  <si>
+    <t>decrement to 0</t>
+  </si>
+  <si>
+    <t>H89_GOT_DATA</t>
+  </si>
+  <si>
+    <t>Checks if CmdFlag = 1</t>
+  </si>
+  <si>
+    <t>Check if = H89_OK_TO_READ</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">if StatusPort = H89_READ_OK </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>return</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> DATA_NOT_READ</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">if true, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>return DATA_NOT_READ</t>
+    </r>
+  </si>
+  <si>
+    <t>H89_OK_TO_READ</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">return </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DATA_SENT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> flag</t>
+    </r>
+  </si>
+  <si>
+    <t>H89_READ_OK</t>
+  </si>
+  <si>
+    <t>Returns data from H89</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Writes status in global currenStatus</t>
+  </si>
 </sst>
 </file>
 
@@ -1030,7 +1235,7 @@
     <numFmt numFmtId="167" formatCode="00"/>
     <numFmt numFmtId="168" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1098,6 +1303,34 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1351,7 +1584,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1583,6 +1816,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1601,6 +1838,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2099,7 +2354,7 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D12" sqref="D12:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2388,17 +2643,17 @@
       <c r="A12" s="83" t="s">
         <v>225</v>
       </c>
-      <c r="B12" s="81">
+      <c r="B12" s="88">
         <v>30</v>
       </c>
-      <c r="C12" s="81" t="s">
-        <v>200</v>
-      </c>
-      <c r="D12" s="89" t="s">
+      <c r="C12" s="88">
+        <v>1</v>
+      </c>
+      <c r="D12" s="91" t="s">
         <v>201</v>
       </c>
-      <c r="E12" s="89"/>
-      <c r="F12" s="89"/>
+      <c r="E12" s="91"/>
+      <c r="F12" s="91"/>
       <c r="G12" s="81"/>
       <c r="H12" s="81"/>
       <c r="I12" s="1"/>
@@ -2407,17 +2662,17 @@
       <c r="A13" s="83" t="s">
         <v>226</v>
       </c>
-      <c r="B13" s="81">
+      <c r="B13" s="88">
         <v>31</v>
       </c>
-      <c r="C13" s="81" t="s">
-        <v>200</v>
-      </c>
-      <c r="D13" s="89" t="s">
+      <c r="C13" s="88">
+        <v>1</v>
+      </c>
+      <c r="D13" s="91" t="s">
         <v>201</v>
       </c>
-      <c r="E13" s="89"/>
-      <c r="F13" s="89"/>
+      <c r="E13" s="91"/>
+      <c r="F13" s="91"/>
       <c r="G13" s="81"/>
       <c r="H13" s="81"/>
       <c r="I13" s="1"/>
@@ -2465,10 +2720,10 @@
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="17"/>
-      <c r="B17" s="87" t="s">
+      <c r="B17" s="89" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="88"/>
+      <c r="C17" s="90"/>
       <c r="D17" s="1"/>
       <c r="H17" s="1"/>
     </row>
@@ -2643,6 +2898,265 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20037C0A-E7AC-4C47-91F4-453F68E8AD73}">
+  <dimension ref="A1:M24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>573</v>
+      </c>
+      <c r="B2">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>245</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>573</v>
+      </c>
+      <c r="D14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>245</v>
+      </c>
+      <c r="D16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>85</v>
+      </c>
+      <c r="E17" t="s">
+        <v>95</v>
+      </c>
+      <c r="M17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>102</v>
+      </c>
+      <c r="I19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>573</v>
+      </c>
+      <c r="D20" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" t="s">
+        <v>99</v>
+      </c>
+      <c r="F20" t="s">
+        <v>88</v>
+      </c>
+      <c r="I20" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" t="s">
+        <v>100</v>
+      </c>
+      <c r="I21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>245</v>
+      </c>
+      <c r="D22" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" t="s">
+        <v>97</v>
+      </c>
+      <c r="F22" t="s">
+        <v>87</v>
+      </c>
+      <c r="G22" t="s">
+        <v>103</v>
+      </c>
+      <c r="I22" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>85</v>
+      </c>
+      <c r="E23" t="s">
+        <v>95</v>
+      </c>
+      <c r="I23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I24" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59EEA5D4-0E1C-4454-AE46-A90AC5C44719}">
   <dimension ref="A1:S38"/>
   <sheetViews>
@@ -3608,60 +4122,330 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B7AA060-9D55-4662-B023-48377CFC4BF5}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:U59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" customWidth="1"/>
+    <col min="11" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="85" t="s">
         <v>230</v>
       </c>
       <c r="B1" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>263</v>
+      </c>
+      <c r="T2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>264</v>
+      </c>
+      <c r="K3">
+        <v>296</v>
+      </c>
+      <c r="L3">
+        <v>4</v>
+      </c>
+      <c r="M3">
+        <v>102</v>
+      </c>
+      <c r="N3">
+        <v>52</v>
+      </c>
+      <c r="O3">
+        <v>52</v>
+      </c>
+      <c r="P3">
+        <v>296</v>
+      </c>
+      <c r="Q3">
+        <v>4</v>
+      </c>
+      <c r="R3">
+        <v>296</v>
+      </c>
+      <c r="S3">
+        <v>296</v>
+      </c>
+      <c r="T3">
+        <v>295</v>
+      </c>
+      <c r="U3">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>265</v>
+      </c>
+      <c r="K4" s="65">
+        <v>36965</v>
+      </c>
+      <c r="L4" s="65">
+        <v>43897</v>
+      </c>
+      <c r="M4">
+        <v>37435</v>
+      </c>
+      <c r="N4">
+        <v>37404</v>
+      </c>
+      <c r="O4">
+        <v>20765</v>
+      </c>
+      <c r="P4">
+        <v>20856</v>
+      </c>
+      <c r="Q4" s="65">
+        <v>43919</v>
+      </c>
+      <c r="R4">
+        <v>37270</v>
+      </c>
+      <c r="S4">
+        <v>36520</v>
+      </c>
+      <c r="T4">
+        <v>37141</v>
+      </c>
+      <c r="U4">
+        <v>37554</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="J5" t="s">
+        <v>266</v>
+      </c>
+      <c r="K5" s="65">
+        <v>89737</v>
+      </c>
+      <c r="L5" s="65">
+        <v>58716</v>
+      </c>
+      <c r="M5">
+        <v>189423</v>
+      </c>
+      <c r="N5">
+        <v>189003</v>
+      </c>
+      <c r="O5">
+        <v>189001</v>
+      </c>
+      <c r="P5">
+        <v>113991</v>
+      </c>
+      <c r="Q5" s="65">
+        <v>58739</v>
+      </c>
+      <c r="R5">
+        <v>113792</v>
+      </c>
+      <c r="S5">
+        <v>94552</v>
+      </c>
+      <c r="T5">
+        <v>97143</v>
+      </c>
+      <c r="U5">
+        <v>95585</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>269</v>
+      </c>
+      <c r="K6" s="65">
+        <f t="shared" ref="K6:U6" si="0">K5-K4</f>
+        <v>52772</v>
+      </c>
+      <c r="L6" s="65">
+        <f t="shared" si="0"/>
+        <v>14819</v>
+      </c>
+      <c r="M6" s="65">
+        <f t="shared" si="0"/>
+        <v>151988</v>
+      </c>
+      <c r="N6" s="65">
+        <f t="shared" si="0"/>
+        <v>151599</v>
+      </c>
+      <c r="O6" s="65">
+        <f t="shared" si="0"/>
+        <v>168236</v>
+      </c>
+      <c r="P6" s="65">
+        <f t="shared" si="0"/>
+        <v>93135</v>
+      </c>
+      <c r="Q6" s="65">
+        <f t="shared" si="0"/>
+        <v>14820</v>
+      </c>
+      <c r="R6" s="65">
+        <f t="shared" si="0"/>
+        <v>76522</v>
+      </c>
+      <c r="S6" s="65">
+        <f t="shared" si="0"/>
+        <v>58032</v>
+      </c>
+      <c r="T6" s="65">
+        <f t="shared" si="0"/>
+        <v>60002</v>
+      </c>
+      <c r="U6" s="65">
+        <f t="shared" si="0"/>
+        <v>58031</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>267</v>
+      </c>
+      <c r="K7" s="87">
+        <f t="shared" ref="K7:U7" si="1">(K6*0.000001)/K3</f>
+        <v>1.7828378378378378E-4</v>
+      </c>
+      <c r="L7" s="87">
+        <f t="shared" si="1"/>
+        <v>3.7047499999999997E-3</v>
+      </c>
+      <c r="M7" s="87">
+        <f t="shared" si="1"/>
+        <v>1.4900784313725489E-3</v>
+      </c>
+      <c r="N7" s="87">
+        <f t="shared" si="1"/>
+        <v>2.9153653846153843E-3</v>
+      </c>
+      <c r="O7" s="87">
+        <f t="shared" si="1"/>
+        <v>3.2353076923076923E-3</v>
+      </c>
+      <c r="P7" s="87">
+        <f t="shared" si="1"/>
+        <v>3.1464527027027026E-4</v>
+      </c>
+      <c r="Q7" s="87">
+        <f t="shared" si="1"/>
+        <v>3.705E-3</v>
+      </c>
+      <c r="R7" s="87">
+        <f t="shared" si="1"/>
+        <v>2.5852027027027023E-4</v>
+      </c>
+      <c r="S7" s="87">
+        <f t="shared" si="1"/>
+        <v>1.9605405405405404E-4</v>
+      </c>
+      <c r="T7" s="87">
+        <f t="shared" si="1"/>
+        <v>2.0339661016949151E-4</v>
+      </c>
+      <c r="U7" s="87">
+        <f t="shared" si="1"/>
+        <v>1.9671525423728813E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="85" t="s">
         <v>231</v>
       </c>
       <c r="B8" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>268</v>
+      </c>
+      <c r="K8" s="65">
+        <f t="shared" ref="K8:U8" si="2">(1/K7)</f>
+        <v>5609.0350943682261</v>
+      </c>
+      <c r="L8" s="65">
+        <f t="shared" si="2"/>
+        <v>269.92374654160204</v>
+      </c>
+      <c r="M8" s="65">
+        <f t="shared" si="2"/>
+        <v>671.10561360107386</v>
+      </c>
+      <c r="N8" s="65">
+        <f t="shared" si="2"/>
+        <v>343.01017816740222</v>
+      </c>
+      <c r="O8" s="65">
+        <f t="shared" si="2"/>
+        <v>309.08961221141732</v>
+      </c>
+      <c r="P8" s="65">
+        <f t="shared" si="2"/>
+        <v>3178.1822086218931</v>
+      </c>
+      <c r="Q8" s="65">
+        <f t="shared" si="2"/>
+        <v>269.90553306342781</v>
+      </c>
+      <c r="R8" s="65">
+        <f t="shared" si="2"/>
+        <v>3868.168631243303</v>
+      </c>
+      <c r="S8" s="65">
+        <f t="shared" si="2"/>
+        <v>5100.6341328921981</v>
+      </c>
+      <c r="T8" s="65">
+        <f t="shared" si="2"/>
+        <v>4916.5027832405585</v>
+      </c>
+      <c r="U8" s="65">
+        <f t="shared" si="2"/>
+        <v>5083.4898588685364</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="M13" s="65"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="M14" s="65"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="85" t="s">
         <v>242</v>
       </c>
       <c r="B16" t="s">
@@ -3699,7 +4483,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="85" t="s">
         <v>243</v>
       </c>
       <c r="B24" t="s">
@@ -3742,7 +4526,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="85" t="s">
         <v>248</v>
       </c>
       <c r="B33" t="s">
@@ -3752,6 +4536,111 @@
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>249</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="85" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="85" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="85" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="85" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="85" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -3761,6 +4650,303 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{221ED582-8995-4CC1-B21C-279F5E9BE25F}">
+  <dimension ref="A1:I48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.28515625" style="96" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" style="97" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="97" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="97" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="97" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" style="97" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" style="97" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="97"/>
+    <col min="9" max="9" width="9.140625" style="96"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="97" t="s">
+        <v>292</v>
+      </c>
+      <c r="C1" s="98" t="s">
+        <v>293</v>
+      </c>
+      <c r="D1" s="97" t="s">
+        <v>294</v>
+      </c>
+      <c r="E1" s="97" t="s">
+        <v>295</v>
+      </c>
+      <c r="F1" s="97" t="s">
+        <v>296</v>
+      </c>
+      <c r="G1" s="97" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="99" t="s">
+        <v>230</v>
+      </c>
+      <c r="B2" s="98"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="97" t="s">
+        <v>232</v>
+      </c>
+      <c r="B3" s="97" t="s">
+        <v>298</v>
+      </c>
+      <c r="C3" s="97" t="s">
+        <v>298</v>
+      </c>
+      <c r="D3" s="97">
+        <v>0</v>
+      </c>
+      <c r="E3" s="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="99" t="s">
+        <v>231</v>
+      </c>
+      <c r="B5" s="98"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="97" t="s">
+        <v>235</v>
+      </c>
+      <c r="B6" s="97" t="s">
+        <v>299</v>
+      </c>
+      <c r="F6" s="97" t="s">
+        <v>300</v>
+      </c>
+      <c r="G6" s="97" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="99" t="s">
+        <v>242</v>
+      </c>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="97" t="s">
+        <v>241</v>
+      </c>
+      <c r="B9" s="97" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="100" t="s">
+        <v>302</v>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="100" t="s">
+        <v>238</v>
+      </c>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="100" t="s">
+        <v>239</v>
+      </c>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="100" t="s">
+        <v>240</v>
+      </c>
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="97" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="99" t="s">
+        <v>243</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="G16" s="97" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+      <c r="A17" s="101" t="s">
+        <v>304</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="G17" s="97" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="97" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="97" t="s">
+        <v>245</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="G19" s="97" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="97" t="s">
+        <v>307</v>
+      </c>
+      <c r="B20" s="97" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="99" t="s">
+        <v>248</v>
+      </c>
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="97" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="99" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="97" t="s">
+        <v>282</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="97" t="s">
+        <v>311</v>
+      </c>
+      <c r="B27" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="99" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="96" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="96" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="96" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="99" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="96" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="96" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="96" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="96" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="99" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="96" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="96" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="96" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="96" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="99" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="96" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="96" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="96" t="s">
+        <v>280</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C8F22C3-4A63-495E-B4FE-DD401B0D152C}">
   <dimension ref="A2:F36"/>
   <sheetViews>
@@ -4299,7 +5485,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6149792-3361-4E66-A023-74FD519AAEBE}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -4344,7 +5530,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8351D32F-052C-49B4-91CF-60F5FD05FC35}">
   <dimension ref="A2:Z49"/>
   <sheetViews>
@@ -4484,16 +5670,16 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="F6" s="2"/>
-      <c r="G6" s="90">
+      <c r="G6" s="92">
         <v>1</v>
       </c>
-      <c r="H6" s="91"/>
-      <c r="I6" s="91"/>
-      <c r="J6" s="90">
+      <c r="H6" s="93"/>
+      <c r="I6" s="93"/>
+      <c r="J6" s="92">
         <v>0</v>
       </c>
-      <c r="K6" s="91"/>
-      <c r="L6" s="91"/>
+      <c r="K6" s="93"/>
+      <c r="L6" s="93"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="X6" s="2" t="s">
@@ -4504,16 +5690,16 @@
       <c r="F7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="92" t="s">
+      <c r="G7" s="94" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="93"/>
-      <c r="I7" s="93"/>
-      <c r="J7" s="92" t="s">
+      <c r="H7" s="95"/>
+      <c r="I7" s="95"/>
+      <c r="J7" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="K7" s="93"/>
-      <c r="L7" s="93"/>
+      <c r="K7" s="95"/>
+      <c r="L7" s="95"/>
       <c r="X7" s="1" t="s">
         <v>66</v>
       </c>
@@ -4528,21 +5714,21 @@
       <c r="F8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="92" t="s">
+      <c r="G8" s="94" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="93"/>
-      <c r="I8" s="93"/>
-      <c r="J8" s="92" t="s">
+      <c r="H8" s="95"/>
+      <c r="I8" s="95"/>
+      <c r="J8" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="K8" s="93"/>
-      <c r="L8" s="93"/>
+      <c r="K8" s="95"/>
+      <c r="L8" s="95"/>
       <c r="O8" s="17"/>
-      <c r="P8" s="87" t="s">
+      <c r="P8" s="89" t="s">
         <v>59</v>
       </c>
-      <c r="Q8" s="88"/>
+      <c r="Q8" s="90"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
       <c r="Y8" s="1" t="s">
@@ -4556,16 +5742,16 @@
       <c r="F9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="92" t="s">
+      <c r="G9" s="94" t="s">
         <v>56</v>
       </c>
-      <c r="H9" s="93"/>
-      <c r="I9" s="93"/>
-      <c r="J9" s="92" t="s">
+      <c r="H9" s="95"/>
+      <c r="I9" s="95"/>
+      <c r="J9" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="K9" s="93"/>
-      <c r="L9" s="93"/>
+      <c r="K9" s="95"/>
+      <c r="L9" s="95"/>
       <c r="O9" s="58" t="s">
         <v>64</v>
       </c>
@@ -4593,16 +5779,16 @@
       <c r="F10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="92" t="s">
+      <c r="G10" s="94" t="s">
         <v>81</v>
       </c>
-      <c r="H10" s="93"/>
-      <c r="I10" s="93"/>
-      <c r="J10" s="92" t="s">
+      <c r="H10" s="95"/>
+      <c r="I10" s="95"/>
+      <c r="J10" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="K10" s="93"/>
-      <c r="L10" s="93"/>
+      <c r="K10" s="95"/>
+      <c r="L10" s="95"/>
       <c r="O10" s="42" t="s">
         <v>60</v>
       </c>
@@ -5122,7 +6308,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E8953BE-283E-447B-901F-738677242859}">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -5225,7 +6411,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{501AD065-09D6-4E30-BC30-53C37491F725}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -5356,7 +6542,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3524476A-77A4-4787-9A72-750F9A8F2315}">
   <dimension ref="A1:L10"/>
   <sheetViews>
@@ -5450,263 +6636,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20037C0A-E7AC-4C47-91F4-453F68E8AD73}">
-  <dimension ref="A1:M24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>573</v>
-      </c>
-      <c r="B2">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E3" t="s">
-        <v>93</v>
-      </c>
-      <c r="G3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E4" t="s">
-        <v>94</v>
-      </c>
-      <c r="F4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>245</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>86</v>
-      </c>
-      <c r="D7" t="s">
-        <v>87</v>
-      </c>
-      <c r="E7" t="s">
-        <v>90</v>
-      </c>
-      <c r="F7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>88</v>
-      </c>
-      <c r="E8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>85</v>
-      </c>
-      <c r="D9" t="s">
-        <v>87</v>
-      </c>
-      <c r="E9" t="s">
-        <v>113</v>
-      </c>
-      <c r="F9">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
-        <v>88</v>
-      </c>
-      <c r="E10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C14">
-        <v>573</v>
-      </c>
-      <c r="D14" t="s">
-        <v>68</v>
-      </c>
-      <c r="E14" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
-        <v>85</v>
-      </c>
-      <c r="E15" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C16">
-        <v>245</v>
-      </c>
-      <c r="D16" t="s">
-        <v>86</v>
-      </c>
-      <c r="E16" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
-        <v>85</v>
-      </c>
-      <c r="E17" t="s">
-        <v>95</v>
-      </c>
-      <c r="M17" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>102</v>
-      </c>
-      <c r="I19" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C20">
-        <v>573</v>
-      </c>
-      <c r="D20" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" t="s">
-        <v>99</v>
-      </c>
-      <c r="F20" t="s">
-        <v>88</v>
-      </c>
-      <c r="I20" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D21" t="s">
-        <v>85</v>
-      </c>
-      <c r="E21" t="s">
-        <v>100</v>
-      </c>
-      <c r="I21" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C22">
-        <v>245</v>
-      </c>
-      <c r="D22" t="s">
-        <v>86</v>
-      </c>
-      <c r="E22" t="s">
-        <v>97</v>
-      </c>
-      <c r="F22" t="s">
-        <v>87</v>
-      </c>
-      <c r="G22" t="s">
-        <v>103</v>
-      </c>
-      <c r="I22" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
-        <v>85</v>
-      </c>
-      <c r="E23" t="s">
-        <v>95</v>
-      </c>
-      <c r="I23" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I24" t="s">
-        <v>107</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
file download temp - not working
</commit_message>
<xml_diff>
--- a/H89_ESP32 Commands.xlsx
+++ b/H89_ESP32 Commands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dev\ESP32\H89_ESP32\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5045C9-E77C-4648-B2B5-C607F2506F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E2B0E2-BB69-417D-93F9-A4FB8403C661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29730" yWindow="3330" windowWidth="21600" windowHeight="11385" tabRatio="636" activeTab="2" xr2:uid="{D2F2CCC8-256C-4E0F-AF5D-63EDFF332B66}"/>
+    <workbookView xWindow="1305" yWindow="1020" windowWidth="27240" windowHeight="13995" tabRatio="636" activeTab="1" xr2:uid="{D2F2CCC8-256C-4E0F-AF5D-63EDFF332B66}"/>
   </bookViews>
   <sheets>
     <sheet name="Cmd Summary" sheetId="8" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="315">
   <si>
     <t>Read Port Function</t>
   </si>
@@ -1221,6 +1221,15 @@
   </si>
   <si>
     <t>Writes status in global currenStatus</t>
+  </si>
+  <si>
+    <t>esp1.pas</t>
+  </si>
+  <si>
+    <t>esp2.pas</t>
+  </si>
+  <si>
+    <t>File List</t>
   </si>
 </sst>
 </file>
@@ -1820,6 +1829,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1827,35 +1854,17 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2649,11 +2658,11 @@
       <c r="C12" s="88">
         <v>1</v>
       </c>
-      <c r="D12" s="91" t="s">
+      <c r="D12" s="97" t="s">
         <v>201</v>
       </c>
-      <c r="E12" s="91"/>
-      <c r="F12" s="91"/>
+      <c r="E12" s="97"/>
+      <c r="F12" s="97"/>
       <c r="G12" s="81"/>
       <c r="H12" s="81"/>
       <c r="I12" s="1"/>
@@ -2668,11 +2677,11 @@
       <c r="C13" s="88">
         <v>1</v>
       </c>
-      <c r="D13" s="91" t="s">
+      <c r="D13" s="97" t="s">
         <v>201</v>
       </c>
-      <c r="E13" s="91"/>
-      <c r="F13" s="91"/>
+      <c r="E13" s="97"/>
+      <c r="F13" s="97"/>
       <c r="G13" s="81"/>
       <c r="H13" s="81"/>
       <c r="I13" s="1"/>
@@ -2720,10 +2729,10 @@
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="17"/>
-      <c r="B17" s="89" t="s">
+      <c r="B17" s="95" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="90"/>
+      <c r="C17" s="96"/>
       <c r="D17" s="1"/>
       <c r="H17" s="1"/>
     </row>
@@ -4122,10 +4131,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B7AA060-9D55-4662-B023-48377CFC4BF5}">
-  <dimension ref="A1:U59"/>
+  <dimension ref="A1:X59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X8" sqref="X8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4134,9 +4143,10 @@
     <col min="10" max="10" width="14.42578125" customWidth="1"/>
     <col min="11" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.85546875" customWidth="1"/>
+    <col min="22" max="23" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="85" t="s">
         <v>230</v>
       </c>
@@ -4144,15 +4154,24 @@
         <v>232</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="K2" t="s">
         <v>263</v>
       </c>
       <c r="T2" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V2" t="s">
+        <v>312</v>
+      </c>
+      <c r="W2" t="s">
+        <v>313</v>
+      </c>
+      <c r="X2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>252</v>
       </c>
@@ -4192,8 +4211,17 @@
       <c r="U3">
         <v>295</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V3">
+        <v>3725</v>
+      </c>
+      <c r="W3">
+        <v>10375</v>
+      </c>
+      <c r="X3">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>233</v>
       </c>
@@ -4233,8 +4261,17 @@
       <c r="U4">
         <v>37554</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V4">
+        <v>14050</v>
+      </c>
+      <c r="W4">
+        <v>14710</v>
+      </c>
+      <c r="X4">
+        <v>63528</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>234</v>
       </c>
@@ -4274,8 +4311,17 @@
       <c r="U5">
         <v>95585</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V5">
+        <v>3064044</v>
+      </c>
+      <c r="W5">
+        <v>8475929</v>
+      </c>
+      <c r="X5">
+        <v>141517</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="J6" t="s">
         <v>269</v>
       </c>
@@ -4323,57 +4369,81 @@
         <f t="shared" si="0"/>
         <v>58031</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V6" s="65">
+        <f t="shared" ref="V6:W6" si="1">V5-V4</f>
+        <v>3049994</v>
+      </c>
+      <c r="W6" s="65">
+        <f t="shared" si="1"/>
+        <v>8461219</v>
+      </c>
+      <c r="X6" s="65">
+        <f t="shared" ref="X6" si="2">X5-X4</f>
+        <v>77989</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="J7" t="s">
         <v>267</v>
       </c>
       <c r="K7" s="87">
-        <f t="shared" ref="K7:U7" si="1">(K6*0.000001)/K3</f>
+        <f t="shared" ref="K7:U7" si="3">(K6*0.000001)/K3</f>
         <v>1.7828378378378378E-4</v>
       </c>
       <c r="L7" s="87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.7047499999999997E-3</v>
       </c>
       <c r="M7" s="87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.4900784313725489E-3</v>
       </c>
       <c r="N7" s="87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.9153653846153843E-3</v>
       </c>
       <c r="O7" s="87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.2353076923076923E-3</v>
       </c>
       <c r="P7" s="87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.1464527027027026E-4</v>
       </c>
       <c r="Q7" s="87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.705E-3</v>
       </c>
       <c r="R7" s="87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.5852027027027023E-4</v>
       </c>
       <c r="S7" s="87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.9605405405405404E-4</v>
       </c>
       <c r="T7" s="87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.0339661016949151E-4</v>
       </c>
       <c r="U7" s="87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.9671525423728813E-4</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V7" s="87">
+        <f t="shared" ref="V7:W7" si="4">(V6*0.000001)/V3</f>
+        <v>8.1879033557046975E-4</v>
+      </c>
+      <c r="W7" s="87">
+        <f t="shared" si="4"/>
+        <v>8.1553918072289151E-4</v>
+      </c>
+      <c r="X7" s="87">
+        <f t="shared" ref="X7" si="5">(X6*0.000001)/X3</f>
+        <v>2.2030790960451979E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="85" t="s">
         <v>231</v>
       </c>
@@ -4384,67 +4454,79 @@
         <v>268</v>
       </c>
       <c r="K8" s="65">
-        <f t="shared" ref="K8:U8" si="2">(1/K7)</f>
+        <f t="shared" ref="K8:U8" si="6">(1/K7)</f>
         <v>5609.0350943682261</v>
       </c>
       <c r="L8" s="65">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>269.92374654160204</v>
       </c>
       <c r="M8" s="65">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>671.10561360107386</v>
       </c>
       <c r="N8" s="65">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>343.01017816740222</v>
       </c>
       <c r="O8" s="65">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>309.08961221141732</v>
       </c>
       <c r="P8" s="65">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>3178.1822086218931</v>
       </c>
       <c r="Q8" s="65">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>269.90553306342781</v>
       </c>
       <c r="R8" s="65">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>3868.168631243303</v>
       </c>
       <c r="S8" s="65">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>5100.6341328921981</v>
       </c>
       <c r="T8" s="65">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>4916.5027832405585</v>
       </c>
       <c r="U8" s="65">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>5083.4898588685364</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V8" s="65">
+        <f t="shared" ref="V8:W8" si="7">(1/V7)</f>
+        <v>1221.3138779945141</v>
+      </c>
+      <c r="W8" s="65">
+        <f t="shared" si="7"/>
+        <v>1226.1826576052458</v>
+      </c>
+      <c r="X8" s="65">
+        <f t="shared" ref="X8" si="8">(1/X7)</f>
+        <v>4539.1016681839747</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="M13" s="65"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="M14" s="65"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="85" t="s">
         <v>242</v>
       </c>
@@ -4653,189 +4735,189 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{221ED582-8995-4CC1-B21C-279F5E9BE25F}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.28515625" style="96" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" style="97" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="97" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="97" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="97" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="97" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" style="97" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="97"/>
-    <col min="9" max="9" width="9.140625" style="96"/>
+    <col min="1" max="1" width="31.28515625" style="89" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" style="90" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="90" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="90" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="90" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" style="90" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" style="90" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="90"/>
+    <col min="9" max="9" width="9.140625" style="89"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="97" t="s">
+      <c r="B1" s="90" t="s">
         <v>292</v>
       </c>
-      <c r="C1" s="98" t="s">
+      <c r="C1" s="91" t="s">
         <v>293</v>
       </c>
-      <c r="D1" s="97" t="s">
+      <c r="D1" s="90" t="s">
         <v>294</v>
       </c>
-      <c r="E1" s="97" t="s">
+      <c r="E1" s="90" t="s">
         <v>295</v>
       </c>
-      <c r="F1" s="97" t="s">
+      <c r="F1" s="90" t="s">
         <v>296</v>
       </c>
-      <c r="G1" s="97" t="s">
+      <c r="G1" s="90" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="92" t="s">
         <v>230</v>
       </c>
-      <c r="B2" s="98"/>
+      <c r="B2" s="91"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="97" t="s">
+      <c r="A3" s="90" t="s">
         <v>232</v>
       </c>
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="90" t="s">
         <v>298</v>
       </c>
-      <c r="C3" s="97" t="s">
+      <c r="C3" s="90" t="s">
         <v>298</v>
       </c>
-      <c r="D3" s="97">
+      <c r="D3" s="90">
         <v>0</v>
       </c>
-      <c r="E3" s="97">
+      <c r="E3" s="90">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="99" t="s">
+      <c r="A5" s="92" t="s">
         <v>231</v>
       </c>
-      <c r="B5" s="98"/>
+      <c r="B5" s="91"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="97" t="s">
+      <c r="A6" s="90" t="s">
         <v>235</v>
       </c>
-      <c r="B6" s="97" t="s">
+      <c r="B6" s="90" t="s">
         <v>299</v>
       </c>
-      <c r="F6" s="97" t="s">
+      <c r="F6" s="90" t="s">
         <v>300</v>
       </c>
-      <c r="G6" s="97" t="s">
+      <c r="G6" s="90" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="99" t="s">
+      <c r="A8" s="92" t="s">
         <v>242</v>
       </c>
       <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="97" t="s">
+      <c r="A9" s="90" t="s">
         <v>241</v>
       </c>
-      <c r="B9" s="97" t="s">
+      <c r="B9" s="90" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="100" t="s">
+      <c r="A10" s="93" t="s">
         <v>302</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="100" t="s">
+      <c r="A11" s="93" t="s">
         <v>238</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="100" t="s">
+      <c r="A12" s="93" t="s">
         <v>239</v>
       </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="100" t="s">
+      <c r="A13" s="93" t="s">
         <v>240</v>
       </c>
       <c r="B13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="97" t="s">
+      <c r="B14" s="90" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="99" t="s">
+      <c r="A16" s="92" t="s">
         <v>243</v>
       </c>
       <c r="B16" s="1"/>
-      <c r="G16" s="97" t="s">
+      <c r="G16" s="90" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="24" x14ac:dyDescent="0.25">
-      <c r="A17" s="101" t="s">
+      <c r="A17" s="94" t="s">
         <v>304</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="G17" s="97" t="s">
+      <c r="G17" s="90" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="97" t="s">
+      <c r="B18" s="90" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="97" t="s">
+      <c r="A19" s="90" t="s">
         <v>245</v>
       </c>
       <c r="B19" s="1"/>
-      <c r="G19" s="97" t="s">
+      <c r="G19" s="90" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="97" t="s">
+      <c r="A20" s="90" t="s">
         <v>307</v>
       </c>
-      <c r="B20" s="97" t="s">
+      <c r="B20" s="90" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="99" t="s">
+      <c r="A22" s="92" t="s">
         <v>248</v>
       </c>
       <c r="B22" s="1"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="97" t="s">
+      <c r="A23" s="90" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="99" t="s">
+      <c r="A25" s="92" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="97" t="s">
+      <c r="A26" s="90" t="s">
         <v>282</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -4846,98 +4928,98 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="97" t="s">
+      <c r="A27" s="90" t="s">
         <v>311</v>
       </c>
       <c r="B27" s="1"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="99" t="s">
+      <c r="A29" s="92" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="96" t="s">
+      <c r="A30" s="89" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="96" t="s">
+      <c r="A31" s="89" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="96" t="s">
+      <c r="A32" s="89" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="99" t="s">
+      <c r="A33" s="92" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="96" t="s">
+      <c r="A34" s="89" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="96" t="s">
+      <c r="A35" s="89" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="96" t="s">
+      <c r="A36" s="89" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="96" t="s">
+      <c r="A37" s="89" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="99" t="s">
+      <c r="A39" s="92" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="96" t="s">
+      <c r="A40" s="89" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="96" t="s">
+      <c r="A41" s="89" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="96" t="s">
+      <c r="A42" s="89" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="96" t="s">
+      <c r="A43" s="89" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="99" t="s">
+      <c r="A45" s="92" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="96" t="s">
+      <c r="A46" s="89" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="96" t="s">
+      <c r="A47" s="89" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="96" t="s">
+      <c r="A48" s="89" t="s">
         <v>280</v>
       </c>
     </row>
@@ -5670,16 +5752,16 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="F6" s="2"/>
-      <c r="G6" s="92">
+      <c r="G6" s="100">
         <v>1</v>
       </c>
-      <c r="H6" s="93"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="92">
+      <c r="H6" s="101"/>
+      <c r="I6" s="101"/>
+      <c r="J6" s="100">
         <v>0</v>
       </c>
-      <c r="K6" s="93"/>
-      <c r="L6" s="93"/>
+      <c r="K6" s="101"/>
+      <c r="L6" s="101"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="X6" s="2" t="s">
@@ -5690,16 +5772,16 @@
       <c r="F7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="94" t="s">
+      <c r="G7" s="98" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="95"/>
-      <c r="I7" s="95"/>
-      <c r="J7" s="94" t="s">
+      <c r="H7" s="99"/>
+      <c r="I7" s="99"/>
+      <c r="J7" s="98" t="s">
         <v>38</v>
       </c>
-      <c r="K7" s="95"/>
-      <c r="L7" s="95"/>
+      <c r="K7" s="99"/>
+      <c r="L7" s="99"/>
       <c r="X7" s="1" t="s">
         <v>66</v>
       </c>
@@ -5714,21 +5796,21 @@
       <c r="F8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="94" t="s">
+      <c r="G8" s="98" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="95"/>
-      <c r="I8" s="95"/>
-      <c r="J8" s="94" t="s">
+      <c r="H8" s="99"/>
+      <c r="I8" s="99"/>
+      <c r="J8" s="98" t="s">
         <v>41</v>
       </c>
-      <c r="K8" s="95"/>
-      <c r="L8" s="95"/>
+      <c r="K8" s="99"/>
+      <c r="L8" s="99"/>
       <c r="O8" s="17"/>
-      <c r="P8" s="89" t="s">
+      <c r="P8" s="95" t="s">
         <v>59</v>
       </c>
-      <c r="Q8" s="90"/>
+      <c r="Q8" s="96"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
       <c r="Y8" s="1" t="s">
@@ -5742,16 +5824,16 @@
       <c r="F9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="94" t="s">
+      <c r="G9" s="98" t="s">
         <v>56</v>
       </c>
-      <c r="H9" s="95"/>
-      <c r="I9" s="95"/>
-      <c r="J9" s="94" t="s">
+      <c r="H9" s="99"/>
+      <c r="I9" s="99"/>
+      <c r="J9" s="98" t="s">
         <v>57</v>
       </c>
-      <c r="K9" s="95"/>
-      <c r="L9" s="95"/>
+      <c r="K9" s="99"/>
+      <c r="L9" s="99"/>
       <c r="O9" s="58" t="s">
         <v>64</v>
       </c>
@@ -5779,16 +5861,16 @@
       <c r="F10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="94" t="s">
+      <c r="G10" s="98" t="s">
         <v>81</v>
       </c>
-      <c r="H10" s="95"/>
-      <c r="I10" s="95"/>
-      <c r="J10" s="94" t="s">
+      <c r="H10" s="99"/>
+      <c r="I10" s="99"/>
+      <c r="J10" s="98" t="s">
         <v>82</v>
       </c>
-      <c r="K10" s="95"/>
-      <c r="L10" s="95"/>
+      <c r="K10" s="99"/>
+      <c r="L10" s="99"/>
       <c r="O10" s="42" t="s">
         <v>60</v>
       </c>
@@ -6287,17 +6369,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="J8:L8"/>
     <mergeCell ref="P8:Q8"/>
     <mergeCell ref="J9:L9"/>
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="G9:I9"/>
     <mergeCell ref="G10:I10"/>
     <mergeCell ref="J10:L10"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="J8:L8"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Working xmodem up and down
</commit_message>
<xml_diff>
--- a/H89_ESP32 Commands.xlsx
+++ b/H89_ESP32 Commands.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dev\ESP32\H89_ESP32\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E2B0E2-BB69-417D-93F9-A4FB8403C661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E57CBD3-A52E-46B6-AEDC-7D044672733F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1305" yWindow="1020" windowWidth="27240" windowHeight="13995" tabRatio="636" activeTab="1" xr2:uid="{D2F2CCC8-256C-4E0F-AF5D-63EDFF332B66}"/>
+    <workbookView xWindow="30435" yWindow="1155" windowWidth="21600" windowHeight="11385" tabRatio="636" xr2:uid="{D2F2CCC8-256C-4E0F-AF5D-63EDFF332B66}"/>
   </bookViews>
   <sheets>
     <sheet name="Cmd Summary" sheetId="8" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="321">
   <si>
     <t>Read Port Function</t>
   </si>
@@ -1230,6 +1230,24 @@
   </si>
   <si>
     <t>File List</t>
+  </si>
+  <si>
+    <t>Download</t>
+  </si>
+  <si>
+    <t>Upload</t>
+  </si>
+  <si>
+    <t>esp3</t>
+  </si>
+  <si>
+    <t>1, 2</t>
+  </si>
+  <si>
+    <t>No Esp32 sector message</t>
+  </si>
+  <si>
+    <t>No H89 sector message</t>
   </si>
 </sst>
 </file>
@@ -1854,17 +1872,17 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2362,8 +2380,8 @@
   </sheetPr>
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12:F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4131,10 +4149,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B7AA060-9D55-4662-B023-48377CFC4BF5}">
-  <dimension ref="A1:X59"/>
+  <dimension ref="A1:AB59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X8" sqref="X8"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4144,17 +4162,37 @@
     <col min="11" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.85546875" customWidth="1"/>
     <col min="22" max="23" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.5703125" customWidth="1"/>
+    <col min="27" max="27" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="85" t="s">
         <v>230</v>
       </c>
       <c r="B1" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="V1" t="s">
+        <v>315</v>
+      </c>
+      <c r="W1" t="s">
+        <v>316</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>316</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>315</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>315</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="K2" t="s">
         <v>263</v>
       </c>
@@ -4170,8 +4208,20 @@
       <c r="X2" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y2" t="s">
+        <v>317</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>317</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>317</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>252</v>
       </c>
@@ -4220,8 +4270,20 @@
       <c r="X3">
         <v>354</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y3">
+        <v>9045</v>
+      </c>
+      <c r="Z3">
+        <v>9045</v>
+      </c>
+      <c r="AA3">
+        <v>9045</v>
+      </c>
+      <c r="AB3">
+        <v>9045</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>233</v>
       </c>
@@ -4271,7 +4333,7 @@
         <v>63528</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>234</v>
       </c>
@@ -4321,7 +4383,7 @@
         <v>141517</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="J6" t="s">
         <v>269</v>
       </c>
@@ -4381,8 +4443,20 @@
         <f t="shared" ref="X6" si="2">X5-X4</f>
         <v>77989</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y6">
+        <v>12758991</v>
+      </c>
+      <c r="Z6">
+        <v>10688967</v>
+      </c>
+      <c r="AA6">
+        <v>10657962</v>
+      </c>
+      <c r="AB6">
+        <v>10323330</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="J7" t="s">
         <v>267</v>
       </c>
@@ -4439,11 +4513,27 @@
         <v>8.1553918072289151E-4</v>
       </c>
       <c r="X7" s="87">
-        <f t="shared" ref="X7" si="5">(X6*0.000001)/X3</f>
+        <f t="shared" ref="X7:Z7" si="5">(X6*0.000001)/X3</f>
         <v>2.2030790960451979E-4</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y7" s="87">
+        <f t="shared" si="5"/>
+        <v>1.4106126036484245E-3</v>
+      </c>
+      <c r="Z7" s="87">
+        <f t="shared" si="5"/>
+        <v>1.1817542288557214E-3</v>
+      </c>
+      <c r="AA7" s="87">
+        <f t="shared" ref="AA7:AB7" si="6">(AA6*0.000001)/AA3</f>
+        <v>1.178326368159204E-3</v>
+      </c>
+      <c r="AB7" s="87">
+        <f t="shared" si="6"/>
+        <v>1.1413300165837479E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="85" t="s">
         <v>231</v>
       </c>
@@ -4454,79 +4544,126 @@
         <v>268</v>
       </c>
       <c r="K8" s="65">
-        <f t="shared" ref="K8:U8" si="6">(1/K7)</f>
+        <f t="shared" ref="K8:U8" si="7">(1/K7)</f>
         <v>5609.0350943682261</v>
       </c>
       <c r="L8" s="65">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>269.92374654160204</v>
       </c>
       <c r="M8" s="65">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>671.10561360107386</v>
       </c>
       <c r="N8" s="65">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>343.01017816740222</v>
       </c>
       <c r="O8" s="65">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>309.08961221141732</v>
       </c>
       <c r="P8" s="65">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3178.1822086218931</v>
       </c>
       <c r="Q8" s="65">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>269.90553306342781</v>
       </c>
       <c r="R8" s="65">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3868.168631243303</v>
       </c>
       <c r="S8" s="65">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5100.6341328921981</v>
       </c>
       <c r="T8" s="65">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4916.5027832405585</v>
       </c>
       <c r="U8" s="65">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5083.4898588685364</v>
       </c>
       <c r="V8" s="65">
-        <f t="shared" ref="V8:W8" si="7">(1/V7)</f>
+        <f t="shared" ref="V8:W8" si="8">(1/V7)</f>
         <v>1221.3138779945141</v>
       </c>
       <c r="W8" s="65">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1226.1826576052458</v>
       </c>
       <c r="X8" s="65">
-        <f t="shared" ref="X8" si="8">(1/X7)</f>
+        <f t="shared" ref="X8:Z8" si="9">(1/X7)</f>
         <v>4539.1016681839747</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y8" s="65">
+        <f t="shared" si="9"/>
+        <v>708.91185674478493</v>
+      </c>
+      <c r="Z8" s="65">
+        <f t="shared" si="9"/>
+        <v>846.19963743923995</v>
+      </c>
+      <c r="AA8" s="65">
+        <f t="shared" ref="AA8:AB8" si="10">(1/AA7)</f>
+        <v>848.66131067083927</v>
+      </c>
+      <c r="AB8" s="65">
+        <f t="shared" si="10"/>
+        <v>876.17077047813063</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>117</v>
+      </c>
+      <c r="X9" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y9">
+        <v>1</v>
+      </c>
+      <c r="AA9">
+        <v>1</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="M13" s="65"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="M14" s="65"/>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X14">
+        <v>1</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="X15">
+        <v>2</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="85" t="s">
         <v>242</v>
       </c>
@@ -4726,6 +4863,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -5616,7 +5754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8351D32F-052C-49B4-91CF-60F5FD05FC35}">
   <dimension ref="A2:Z49"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O8" sqref="O8:S14"/>
     </sheetView>
   </sheetViews>
@@ -5752,16 +5890,16 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="F6" s="2"/>
-      <c r="G6" s="100">
+      <c r="G6" s="98">
         <v>1</v>
       </c>
-      <c r="H6" s="101"/>
-      <c r="I6" s="101"/>
-      <c r="J6" s="100">
+      <c r="H6" s="99"/>
+      <c r="I6" s="99"/>
+      <c r="J6" s="98">
         <v>0</v>
       </c>
-      <c r="K6" s="101"/>
-      <c r="L6" s="101"/>
+      <c r="K6" s="99"/>
+      <c r="L6" s="99"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="X6" s="2" t="s">
@@ -5772,16 +5910,16 @@
       <c r="F7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="98" t="s">
+      <c r="G7" s="100" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="99"/>
-      <c r="I7" s="99"/>
-      <c r="J7" s="98" t="s">
+      <c r="H7" s="101"/>
+      <c r="I7" s="101"/>
+      <c r="J7" s="100" t="s">
         <v>38</v>
       </c>
-      <c r="K7" s="99"/>
-      <c r="L7" s="99"/>
+      <c r="K7" s="101"/>
+      <c r="L7" s="101"/>
       <c r="X7" s="1" t="s">
         <v>66</v>
       </c>
@@ -5796,16 +5934,16 @@
       <c r="F8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="98" t="s">
+      <c r="G8" s="100" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="99"/>
-      <c r="I8" s="99"/>
-      <c r="J8" s="98" t="s">
+      <c r="H8" s="101"/>
+      <c r="I8" s="101"/>
+      <c r="J8" s="100" t="s">
         <v>41</v>
       </c>
-      <c r="K8" s="99"/>
-      <c r="L8" s="99"/>
+      <c r="K8" s="101"/>
+      <c r="L8" s="101"/>
       <c r="O8" s="17"/>
       <c r="P8" s="95" t="s">
         <v>59</v>
@@ -5824,16 +5962,16 @@
       <c r="F9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="98" t="s">
+      <c r="G9" s="100" t="s">
         <v>56</v>
       </c>
-      <c r="H9" s="99"/>
-      <c r="I9" s="99"/>
-      <c r="J9" s="98" t="s">
+      <c r="H9" s="101"/>
+      <c r="I9" s="101"/>
+      <c r="J9" s="100" t="s">
         <v>57</v>
       </c>
-      <c r="K9" s="99"/>
-      <c r="L9" s="99"/>
+      <c r="K9" s="101"/>
+      <c r="L9" s="101"/>
       <c r="O9" s="58" t="s">
         <v>64</v>
       </c>
@@ -5861,16 +5999,16 @@
       <c r="F10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="98" t="s">
+      <c r="G10" s="100" t="s">
         <v>81</v>
       </c>
-      <c r="H10" s="99"/>
-      <c r="I10" s="99"/>
-      <c r="J10" s="98" t="s">
+      <c r="H10" s="101"/>
+      <c r="I10" s="101"/>
+      <c r="J10" s="100" t="s">
         <v>82</v>
       </c>
-      <c r="K10" s="99"/>
-      <c r="L10" s="99"/>
+      <c r="K10" s="101"/>
+      <c r="L10" s="101"/>
       <c r="O10" s="42" t="s">
         <v>60</v>
       </c>
@@ -6369,17 +6507,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="J8:L8"/>
     <mergeCell ref="P8:Q8"/>
     <mergeCell ref="J9:L9"/>
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="G9:I9"/>
     <mergeCell ref="G10:I10"/>
     <mergeCell ref="J10:L10"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="J8:L8"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
June 13 2023 Xmodem initial byte fix
</commit_message>
<xml_diff>
--- a/H89_ESP32 Commands.xlsx
+++ b/H89_ESP32 Commands.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dev\ESP32\H89_ESP32\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E57CBD3-A52E-46B6-AEDC-7D044672733F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7262E1E7-9A68-4FAE-962E-211CBCBF81AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30435" yWindow="1155" windowWidth="21600" windowHeight="11385" tabRatio="636" xr2:uid="{D2F2CCC8-256C-4E0F-AF5D-63EDFF332B66}"/>
+    <workbookView xWindow="30720" yWindow="1635" windowWidth="26055" windowHeight="13215" tabRatio="636" firstSheet="1" activeTab="12" xr2:uid="{D2F2CCC8-256C-4E0F-AF5D-63EDFF332B66}"/>
   </bookViews>
   <sheets>
     <sheet name="Cmd Summary" sheetId="8" r:id="rId1"/>
@@ -19,15 +19,17 @@
     <sheet name="ESP32 Pins" sheetId="6" r:id="rId4"/>
     <sheet name="PCB Notes" sheetId="10" r:id="rId5"/>
     <sheet name="Commands" sheetId="1" r:id="rId6"/>
-    <sheet name="Timing" sheetId="4" r:id="rId7"/>
-    <sheet name="Breadboard" sheetId="3" r:id="rId8"/>
-    <sheet name="LM317T" sheetId="2" r:id="rId9"/>
-    <sheet name="573 245 " sheetId="5" r:id="rId10"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId11"/>
+    <sheet name="Cmd Time" sheetId="12" r:id="rId7"/>
+    <sheet name="Timing" sheetId="4" r:id="rId8"/>
+    <sheet name="Breadboard" sheetId="3" r:id="rId9"/>
+    <sheet name="LM317T" sheetId="2" r:id="rId10"/>
+    <sheet name="573 245 " sheetId="5" r:id="rId11"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId12"/>
+    <sheet name="Sheet3" sheetId="13" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Cmd Summary'!$A$1:$G$22</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="5">Commands!$A$1:$U$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">Commands!$A$1:$U$36</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="342">
   <si>
     <t>Read Port Function</t>
   </si>
@@ -1248,6 +1250,69 @@
   </si>
   <si>
     <t>No H89 sector message</t>
+  </si>
+  <si>
+    <t>Time Us</t>
+  </si>
+  <si>
+    <t>H89 clk 8</t>
+  </si>
+  <si>
+    <t>H89 clk cycle 8Mhz</t>
+  </si>
+  <si>
+    <t>ESP32 sets status Write OK</t>
+  </si>
+  <si>
+    <t>Writes data 7C</t>
+  </si>
+  <si>
+    <t>Set status</t>
+  </si>
+  <si>
+    <t>Start data Read</t>
+  </si>
+  <si>
+    <t>End data Read</t>
+  </si>
+  <si>
+    <t>Time to read 8 bits data</t>
+  </si>
+  <si>
+    <t>Time to wake up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debug timing. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cmd Start </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cmd End </t>
+  </si>
+  <si>
+    <t>Port Change</t>
+  </si>
+  <si>
+    <t>Got String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USec/Byte </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cmd Loop time </t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>u sec</t>
+  </si>
+  <si>
+    <t>Sec</t>
+  </si>
+  <si>
+    <t>Minutes</t>
   </si>
 </sst>
 </file>
@@ -1611,7 +1676,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1712,27 +1777,12 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1765,19 +1815,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1788,12 +1834,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1819,17 +1859,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1838,7 +1875,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1865,13 +1901,21 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1881,9 +1925,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2380,13 +2428,13 @@
   </sheetPr>
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" style="72" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" style="63" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" customWidth="1"/>
     <col min="6" max="6" width="12.140625" customWidth="1"/>
@@ -2402,7 +2450,7 @@
       <c r="B1" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="54" t="s">
         <v>191</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -2423,72 +2471,72 @@
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="56" t="s">
         <v>171</v>
       </c>
-      <c r="B2" s="64">
+      <c r="B2" s="57">
         <v>3</v>
       </c>
-      <c r="C2" s="64">
+      <c r="C2" s="57">
         <v>1</v>
       </c>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="63" t="s">
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="56" t="s">
         <v>193</v>
       </c>
-      <c r="H2" s="61"/>
+      <c r="H2" s="9"/>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="56" t="s">
         <v>172</v>
       </c>
-      <c r="B3" s="64">
+      <c r="B3" s="57">
         <v>8</v>
       </c>
-      <c r="C3" s="64">
+      <c r="C3" s="57">
         <v>4</v>
       </c>
-      <c r="D3" s="62" t="s">
+      <c r="D3" s="55" t="s">
         <v>207</v>
       </c>
-      <c r="E3" s="62" t="s">
+      <c r="E3" s="55" t="s">
         <v>208</v>
       </c>
-      <c r="F3" s="62" t="s">
+      <c r="F3" s="55" t="s">
         <v>204</v>
       </c>
-      <c r="G3" s="63" t="s">
+      <c r="G3" s="56" t="s">
         <v>184</v>
       </c>
-      <c r="H3" s="61"/>
+      <c r="H3" s="9"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="63" t="s">
+      <c r="A4" s="56" t="s">
         <v>173</v>
       </c>
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="57" t="s">
         <v>198</v>
       </c>
-      <c r="C4" s="64">
+      <c r="C4" s="57">
         <v>4</v>
       </c>
-      <c r="D4" s="62" t="s">
+      <c r="D4" s="55" t="s">
         <v>207</v>
       </c>
-      <c r="E4" s="62" t="s">
+      <c r="E4" s="55" t="s">
         <v>208</v>
       </c>
-      <c r="F4" s="62" t="s">
+      <c r="F4" s="55" t="s">
         <v>209</v>
       </c>
-      <c r="G4" s="63" t="s">
+      <c r="G4" s="56" t="s">
         <v>194</v>
       </c>
-      <c r="H4" s="61"/>
+      <c r="H4" s="9"/>
       <c r="I4" s="1"/>
       <c r="K4">
         <v>1024</v>
@@ -2499,7 +2547,7 @@
       <c r="M4">
         <v>8</v>
       </c>
-      <c r="N4" s="65">
+      <c r="N4" s="58">
         <f>K4*L4*M4</f>
         <v>8388608</v>
       </c>
@@ -2508,14 +2556,14 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="67"/>
-      <c r="B5" s="64"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="66"/>
+      <c r="A5" s="56"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="9"/>
       <c r="I5" s="1"/>
       <c r="N5">
         <f>L4*M4</f>
@@ -2526,22 +2574,22 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="67" t="s">
+      <c r="A6" s="56" t="s">
         <v>178</v>
       </c>
-      <c r="B6" s="64">
+      <c r="B6" s="57">
         <v>10</v>
       </c>
-      <c r="C6" s="64">
+      <c r="C6" s="57">
         <v>1</v>
       </c>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="67" t="s">
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="56" t="s">
         <v>195</v>
       </c>
-      <c r="H6" s="66"/>
+      <c r="H6" s="9"/>
       <c r="I6" s="1"/>
       <c r="K6">
         <v>256</v>
@@ -2555,26 +2603,26 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="67" t="s">
+      <c r="A7" s="56" t="s">
         <v>179</v>
       </c>
-      <c r="B7" s="64">
+      <c r="B7" s="57">
         <v>11</v>
       </c>
-      <c r="C7" s="64" t="s">
+      <c r="C7" s="57" t="s">
         <v>200</v>
       </c>
-      <c r="D7" s="62" t="s">
+      <c r="D7" s="55" t="s">
         <v>219</v>
       </c>
-      <c r="E7" s="67" t="s">
+      <c r="E7" s="56" t="s">
         <v>201</v>
       </c>
-      <c r="F7" s="67"/>
-      <c r="G7" s="73" t="s">
+      <c r="F7" s="56"/>
+      <c r="G7" s="64" t="s">
         <v>196</v>
       </c>
-      <c r="H7" s="66"/>
+      <c r="H7" s="9"/>
       <c r="I7" s="1"/>
       <c r="K7">
         <v>2</v>
@@ -2588,239 +2636,239 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="67" t="s">
+      <c r="A8" s="56" t="s">
         <v>179</v>
       </c>
-      <c r="B8" s="64">
+      <c r="B8" s="57">
         <v>12</v>
       </c>
-      <c r="C8" s="64">
+      <c r="C8" s="57">
         <v>3</v>
       </c>
-      <c r="D8" s="62" t="s">
+      <c r="D8" s="55" t="s">
         <v>219</v>
       </c>
-      <c r="E8" s="68" t="s">
+      <c r="E8" s="59" t="s">
         <v>202</v>
       </c>
-      <c r="F8" s="69"/>
-      <c r="G8" s="73" t="s">
+      <c r="F8" s="60"/>
+      <c r="G8" s="64" t="s">
         <v>196</v>
       </c>
-      <c r="H8" s="66"/>
+      <c r="H8" s="9"/>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="67" t="s">
+      <c r="A9" s="56" t="s">
         <v>172</v>
       </c>
-      <c r="B9" s="64">
+      <c r="B9" s="57">
         <v>28</v>
       </c>
-      <c r="C9" s="64">
+      <c r="C9" s="57">
         <v>4</v>
       </c>
-      <c r="D9" s="62" t="s">
+      <c r="D9" s="55" t="s">
         <v>221</v>
       </c>
-      <c r="E9" s="62" t="s">
+      <c r="E9" s="55" t="s">
         <v>203</v>
       </c>
-      <c r="F9" s="62" t="s">
+      <c r="F9" s="55" t="s">
         <v>204</v>
       </c>
-      <c r="G9" s="67" t="s">
+      <c r="G9" s="56" t="s">
         <v>184</v>
       </c>
-      <c r="H9" s="67"/>
+      <c r="H9" s="56"/>
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="67" t="s">
+      <c r="A10" s="56" t="s">
         <v>173</v>
       </c>
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="57" t="s">
         <v>199</v>
       </c>
-      <c r="C10" s="64">
+      <c r="C10" s="57">
         <v>4</v>
       </c>
-      <c r="D10" s="62" t="s">
+      <c r="D10" s="55" t="s">
         <v>221</v>
       </c>
-      <c r="E10" s="62" t="s">
+      <c r="E10" s="55" t="s">
         <v>203</v>
       </c>
-      <c r="F10" s="62" t="s">
+      <c r="F10" s="55" t="s">
         <v>204</v>
       </c>
-      <c r="G10" s="67" t="s">
+      <c r="G10" s="56" t="s">
         <v>194</v>
       </c>
-      <c r="H10" s="67"/>
+      <c r="H10" s="56"/>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="D11" s="74" t="s">
+      <c r="D11" s="65" t="s">
         <v>222</v>
       </c>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="83" t="s">
+      <c r="A12" s="73" t="s">
         <v>225</v>
       </c>
-      <c r="B12" s="88">
+      <c r="B12" s="77">
         <v>30</v>
       </c>
-      <c r="C12" s="88">
+      <c r="C12" s="77">
         <v>1</v>
       </c>
-      <c r="D12" s="97" t="s">
+      <c r="D12" s="90" t="s">
         <v>201</v>
       </c>
-      <c r="E12" s="97"/>
-      <c r="F12" s="97"/>
-      <c r="G12" s="81"/>
-      <c r="H12" s="81"/>
+      <c r="E12" s="90"/>
+      <c r="F12" s="90"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="71"/>
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="83" t="s">
+      <c r="A13" s="73" t="s">
         <v>226</v>
       </c>
-      <c r="B13" s="88">
+      <c r="B13" s="77">
         <v>31</v>
       </c>
-      <c r="C13" s="88">
+      <c r="C13" s="77">
         <v>1</v>
       </c>
-      <c r="D13" s="97" t="s">
+      <c r="D13" s="90" t="s">
         <v>201</v>
       </c>
-      <c r="E13" s="97"/>
-      <c r="F13" s="97"/>
-      <c r="G13" s="81"/>
-      <c r="H13" s="81"/>
+      <c r="E13" s="90"/>
+      <c r="F13" s="90"/>
+      <c r="G13" s="71"/>
+      <c r="H13" s="71"/>
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="75" t="s">
+      <c r="A14" s="66" t="s">
         <v>223</v>
       </c>
-      <c r="B14" s="82">
+      <c r="B14" s="72">
         <v>1</v>
       </c>
-      <c r="C14" s="77">
+      <c r="C14" s="68">
         <v>4</v>
       </c>
-      <c r="D14" s="78" t="s">
+      <c r="D14" s="69" t="s">
         <v>182</v>
       </c>
-      <c r="E14" s="79" t="s">
+      <c r="E14" s="70" t="s">
         <v>182</v>
       </c>
-      <c r="F14" s="76" t="s">
+      <c r="F14" s="67" t="s">
         <v>182</v>
       </c>
-      <c r="G14" s="80" t="s">
+      <c r="G14" s="69" t="s">
         <v>224</v>
       </c>
-      <c r="H14" s="81"/>
+      <c r="H14" s="71"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="83" t="s">
+      <c r="A15" s="73" t="s">
         <v>229</v>
       </c>
-      <c r="B15" s="84">
+      <c r="B15" s="71">
         <v>0</v>
       </c>
-      <c r="C15" s="81">
+      <c r="C15" s="71">
         <v>1</v>
       </c>
-      <c r="D15" s="81"/>
-      <c r="E15" s="81"/>
-      <c r="F15" s="81"/>
-      <c r="G15" s="81"/>
-      <c r="H15" s="81"/>
+      <c r="D15" s="71"/>
+      <c r="E15" s="71"/>
+      <c r="F15" s="71"/>
+      <c r="G15" s="71"/>
+      <c r="H15" s="71"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="17"/>
-      <c r="B17" s="95" t="s">
+      <c r="B17" s="88" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="96"/>
+      <c r="C17" s="89"/>
       <c r="D17" s="1"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="58" t="s">
+      <c r="A18" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="59">
+      <c r="B18" s="53">
         <v>1</v>
       </c>
-      <c r="C18" s="59">
+      <c r="C18" s="53">
         <v>0</v>
       </c>
-      <c r="D18" s="54" t="s">
+      <c r="D18" s="49" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="43">
+      <c r="B19" s="19">
         <v>0</v>
       </c>
-      <c r="C19" s="43">
+      <c r="C19" s="19">
         <v>0</v>
       </c>
-      <c r="D19" s="45">
+      <c r="D19" s="40">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="46" t="s">
+      <c r="A20" s="41" t="s">
         <v>148</v>
       </c>
-      <c r="B20" s="43">
+      <c r="B20" s="19">
         <v>0</v>
       </c>
-      <c r="C20" s="43">
+      <c r="C20" s="19">
         <v>1</v>
       </c>
-      <c r="D20" s="45">
+      <c r="D20" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="47" t="s">
+      <c r="A21" s="42" t="s">
         <v>149</v>
       </c>
-      <c r="B21" s="43">
+      <c r="B21" s="19">
         <v>1</v>
       </c>
-      <c r="C21" s="43">
+      <c r="C21" s="19">
         <v>0</v>
       </c>
-      <c r="D21" s="45">
+      <c r="D21" s="40">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="48" t="s">
+      <c r="A22" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="49">
+      <c r="B22" s="44">
         <v>1</v>
       </c>
-      <c r="C22" s="49">
+      <c r="C22" s="44">
         <v>1</v>
       </c>
-      <c r="D22" s="51">
+      <c r="D22" s="46">
         <v>3</v>
       </c>
     </row>
@@ -2832,7 +2880,7 @@
       <c r="M23" s="19"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C28" s="70" t="s">
+      <c r="C28" s="61" t="s">
         <v>210</v>
       </c>
     </row>
@@ -2855,7 +2903,7 @@
       <c r="C31" t="s">
         <v>220</v>
       </c>
-      <c r="D31" s="71">
+      <c r="D31" s="62">
         <f>N4</f>
         <v>8388608</v>
       </c>
@@ -2907,7 +2955,7 @@
       <c r="C35" t="s">
         <v>214</v>
       </c>
-      <c r="D35" s="65">
+      <c r="D35" s="58">
         <f>D30*64+D31/POWER(2,D32)+D33</f>
         <v>1048706</v>
       </c>
@@ -2925,6 +2973,102 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3524476A-77A4-4787-9A72-750F9A8F2315}">
+  <dimension ref="A1:L10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2"/>
+      <c r="E2"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="11">
+        <f>1.25*(1+B5/B6)</f>
+        <v>3.125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="B5" s="10">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="B6" s="10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="L8"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="12">
+        <f>B8/(B5+B6)*1000000</f>
+        <v>3300</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20037C0A-E7AC-4C47-91F4-453F68E8AD73}">
   <dimension ref="A1:M24"/>
   <sheetViews>
@@ -3183,7 +3327,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59EEA5D4-0E1C-4454-AE46-A90AC5C44719}">
   <dimension ref="A1:S38"/>
   <sheetViews>
@@ -3194,7 +3338,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="14" style="22" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="38"/>
+    <col min="4" max="4" width="9.140625" style="22"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -3236,7 +3380,7 @@
         <f>REPT(0,8-LEN(DEC2BIN(A3)))&amp;DEC2BIN(A3)</f>
         <v>00000001</v>
       </c>
-      <c r="D3" s="39" t="str">
+      <c r="D3" s="37" t="str">
         <f>REPT(0,8-LEN(DEC2BIN(B3)))&amp;DEC2BIN(B3)</f>
         <v>10000001</v>
       </c>
@@ -3274,7 +3418,7 @@
         <f t="shared" ref="C4:C19" si="0">REPT(0,8-LEN(DEC2BIN(A4)))&amp;DEC2BIN(A4)</f>
         <v>00000101</v>
       </c>
-      <c r="D4" s="39" t="str">
+      <c r="D4" s="37" t="str">
         <f t="shared" ref="D4:D19" si="1">REPT(0,8-LEN(DEC2BIN(B4)))&amp;DEC2BIN(B4)</f>
         <v>10000101</v>
       </c>
@@ -3314,7 +3458,7 @@
         <f t="shared" si="0"/>
         <v>00010010</v>
       </c>
-      <c r="D5" s="39" t="str">
+      <c r="D5" s="37" t="str">
         <f t="shared" si="1"/>
         <v>10010010</v>
       </c>
@@ -3351,7 +3495,7 @@
         <f t="shared" si="0"/>
         <v>00101100</v>
       </c>
-      <c r="D6" s="39" t="str">
+      <c r="D6" s="37" t="str">
         <f t="shared" si="1"/>
         <v>10101100</v>
       </c>
@@ -3394,7 +3538,7 @@
         <f t="shared" si="0"/>
         <v>00000000</v>
       </c>
-      <c r="D7" s="39" t="str">
+      <c r="D7" s="37" t="str">
         <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
@@ -3437,11 +3581,11 @@
         <f t="shared" si="0"/>
         <v>00000110</v>
       </c>
-      <c r="D8" s="39" t="str">
+      <c r="D8" s="37" t="str">
         <f t="shared" si="1"/>
         <v>01010000</v>
       </c>
-      <c r="E8" s="56" t="s">
+      <c r="E8" s="51" t="s">
         <v>166</v>
       </c>
       <c r="H8">
@@ -3483,11 +3627,11 @@
         <f t="shared" si="0"/>
         <v>00001011</v>
       </c>
-      <c r="D9" s="38" t="str">
+      <c r="D9" s="22" t="str">
         <f t="shared" si="1"/>
         <v>01010000</v>
       </c>
-      <c r="E9" s="56" t="s">
+      <c r="E9" s="51" t="s">
         <v>165</v>
       </c>
       <c r="H9">
@@ -3529,11 +3673,11 @@
         <f t="shared" si="0"/>
         <v>00011001</v>
       </c>
-      <c r="D10" s="38" t="str">
+      <c r="D10" s="22" t="str">
         <f t="shared" si="1"/>
         <v>11011000</v>
       </c>
-      <c r="E10" s="56" t="s">
+      <c r="E10" s="51" t="s">
         <v>163</v>
       </c>
       <c r="L10">
@@ -3559,7 +3703,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="55">
+      <c r="A11" s="50">
         <v>52</v>
       </c>
       <c r="B11">
@@ -3569,11 +3713,11 @@
         <f t="shared" si="0"/>
         <v>00110100</v>
       </c>
-      <c r="D11" s="38" t="str">
+      <c r="D11" s="22" t="str">
         <f t="shared" si="1"/>
         <v>10011100</v>
       </c>
-      <c r="E11" s="56" t="s">
+      <c r="E11" s="51" t="s">
         <v>164</v>
       </c>
     </row>
@@ -3588,7 +3732,7 @@
         <f t="shared" si="0"/>
         <v>00000100</v>
       </c>
-      <c r="D12" s="38" t="str">
+      <c r="D12" s="22" t="str">
         <f t="shared" si="1"/>
         <v>00010100</v>
       </c>
@@ -3604,7 +3748,7 @@
         <f t="shared" si="0"/>
         <v>00000101</v>
       </c>
-      <c r="D13" s="38" t="str">
+      <c r="D13" s="22" t="str">
         <f t="shared" si="1"/>
         <v>00010101</v>
       </c>
@@ -3620,13 +3764,13 @@
         <f t="shared" si="0"/>
         <v>00000110</v>
       </c>
-      <c r="D14" s="38" t="str">
+      <c r="D14" s="22" t="str">
         <f t="shared" si="1"/>
         <v>00010110</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="55">
+      <c r="A15" s="50">
         <v>7</v>
       </c>
       <c r="B15">
@@ -3636,7 +3780,7 @@
         <f t="shared" si="0"/>
         <v>00000111</v>
       </c>
-      <c r="D15" s="38" t="str">
+      <c r="D15" s="22" t="str">
         <f t="shared" si="1"/>
         <v>00010111</v>
       </c>
@@ -3652,7 +3796,7 @@
         <f t="shared" si="0"/>
         <v>00001000</v>
       </c>
-      <c r="D16" s="38" t="str">
+      <c r="D16" s="22" t="str">
         <f t="shared" si="1"/>
         <v>00011000</v>
       </c>
@@ -3682,7 +3826,7 @@
         <f t="shared" si="0"/>
         <v>00001001</v>
       </c>
-      <c r="D17" s="38" t="str">
+      <c r="D17" s="22" t="str">
         <f t="shared" si="1"/>
         <v>00011001</v>
       </c>
@@ -3708,7 +3852,7 @@
         <f t="shared" si="0"/>
         <v>00001010</v>
       </c>
-      <c r="D18" s="38" t="str">
+      <c r="D18" s="22" t="str">
         <f t="shared" si="1"/>
         <v>00011010</v>
       </c>
@@ -3731,7 +3875,7 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="55">
+      <c r="A19" s="50">
         <v>11</v>
       </c>
       <c r="B19">
@@ -3741,7 +3885,7 @@
         <f t="shared" si="0"/>
         <v>00001011</v>
       </c>
-      <c r="D19" s="38" t="str">
+      <c r="D19" s="22" t="str">
         <f t="shared" si="1"/>
         <v>00011011</v>
       </c>
@@ -3821,7 +3965,7 @@
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="57">
+      <c r="A23">
         <v>2</v>
       </c>
       <c r="B23">
@@ -3831,7 +3975,7 @@
         <f t="shared" ref="C23:C34" si="6">REPT(0,8-LEN(DEC2BIN(A23)))&amp;DEC2BIN(A23)</f>
         <v>00000010</v>
       </c>
-      <c r="D23" s="38" t="str">
+      <c r="D23" s="22" t="str">
         <f t="shared" ref="D23:D34" si="7">REPT(0,8-LEN(DEC2BIN(B23)))&amp;DEC2BIN(B23)</f>
         <v>01010000</v>
       </c>
@@ -3847,7 +3991,7 @@
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="57">
+      <c r="A24">
         <v>6</v>
       </c>
       <c r="B24">
@@ -3857,7 +4001,7 @@
         <f t="shared" si="6"/>
         <v>00000110</v>
       </c>
-      <c r="D24" s="38" t="str">
+      <c r="D24" s="22" t="str">
         <f t="shared" si="7"/>
         <v>01010000</v>
       </c>
@@ -3870,7 +4014,7 @@
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="57">
+      <c r="A25">
         <v>19</v>
       </c>
       <c r="B25">
@@ -3880,7 +4024,7 @@
         <f t="shared" si="6"/>
         <v>00010011</v>
       </c>
-      <c r="D25" s="38" t="str">
+      <c r="D25" s="22" t="str">
         <f t="shared" si="7"/>
         <v>11011000</v>
       </c>
@@ -3893,7 +4037,7 @@
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="57">
+      <c r="A26">
         <v>45</v>
       </c>
       <c r="B26">
@@ -3903,7 +4047,7 @@
         <f t="shared" si="6"/>
         <v>00101101</v>
       </c>
-      <c r="D26" s="38" t="str">
+      <c r="D26" s="22" t="str">
         <f t="shared" si="7"/>
         <v>10110100</v>
       </c>
@@ -3922,7 +4066,7 @@
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="57">
+      <c r="A27">
         <f>A23+1</f>
         <v>3</v>
       </c>
@@ -3933,7 +4077,7 @@
         <f t="shared" si="6"/>
         <v>00000011</v>
       </c>
-      <c r="D27" s="38" t="str">
+      <c r="D27" s="22" t="str">
         <f t="shared" si="7"/>
         <v>11010000</v>
       </c>
@@ -3952,7 +4096,7 @@
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" s="57">
+      <c r="A28">
         <f t="shared" ref="A28:A38" si="8">A24+1</f>
         <v>7</v>
       </c>
@@ -3963,7 +4107,7 @@
         <f t="shared" si="6"/>
         <v>00000111</v>
       </c>
-      <c r="D28" s="38" t="str">
+      <c r="D28" s="22" t="str">
         <f t="shared" si="7"/>
         <v>11010000</v>
       </c>
@@ -3972,7 +4116,7 @@
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="57">
+      <c r="A29">
         <f t="shared" si="8"/>
         <v>20</v>
       </c>
@@ -3983,7 +4127,7 @@
         <f t="shared" si="6"/>
         <v>00010100</v>
       </c>
-      <c r="D29" s="38" t="str">
+      <c r="D29" s="22" t="str">
         <f t="shared" si="7"/>
         <v>00011000</v>
       </c>
@@ -3992,7 +4136,7 @@
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="57">
+      <c r="A30">
         <f t="shared" si="8"/>
         <v>46</v>
       </c>
@@ -4003,13 +4147,13 @@
         <f t="shared" si="6"/>
         <v>00101110</v>
       </c>
-      <c r="D30" s="38" t="str">
+      <c r="D30" s="22" t="str">
         <f t="shared" si="7"/>
         <v>01110100</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="57">
+      <c r="A31">
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
@@ -4020,13 +4164,13 @@
         <f t="shared" si="6"/>
         <v>00000100</v>
       </c>
-      <c r="D31" s="38" t="str">
+      <c r="D31" s="22" t="str">
         <f t="shared" si="7"/>
         <v>00010000</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="57">
+      <c r="A32">
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
@@ -4037,13 +4181,13 @@
         <f t="shared" si="6"/>
         <v>00001000</v>
       </c>
-      <c r="D32" s="38" t="str">
+      <c r="D32" s="22" t="str">
         <f t="shared" si="7"/>
         <v>10011000</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="57">
+      <c r="A33">
         <f t="shared" si="8"/>
         <v>21</v>
       </c>
@@ -4054,13 +4198,13 @@
         <f t="shared" si="6"/>
         <v>00010101</v>
       </c>
-      <c r="D33" s="38" t="str">
+      <c r="D33" s="22" t="str">
         <f t="shared" si="7"/>
         <v>11110100</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="57">
+      <c r="A34">
         <f t="shared" si="8"/>
         <v>47</v>
       </c>
@@ -4068,13 +4212,13 @@
         <f t="shared" si="6"/>
         <v>00101111</v>
       </c>
-      <c r="D34" s="38" t="str">
+      <c r="D34" s="22" t="str">
         <f t="shared" si="7"/>
         <v>00000000</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="57">
+      <c r="A35">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
@@ -4085,13 +4229,13 @@
         <f t="shared" ref="C35:C38" si="9">REPT(0,8-LEN(DEC2BIN(A35)))&amp;DEC2BIN(A35)</f>
         <v>00000101</v>
       </c>
-      <c r="D35" s="38" t="str">
+      <c r="D35" s="22" t="str">
         <f t="shared" ref="D35:D38" si="10">REPT(0,8-LEN(DEC2BIN(B35)))&amp;DEC2BIN(B35)</f>
         <v>10010000</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="57">
+      <c r="A36">
         <f t="shared" si="8"/>
         <v>9</v>
       </c>
@@ -4102,13 +4246,13 @@
         <f t="shared" si="9"/>
         <v>00001001</v>
       </c>
-      <c r="D36" s="38" t="str">
+      <c r="D36" s="22" t="str">
         <f t="shared" si="10"/>
         <v>10010000</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="57">
+      <c r="A37">
         <f t="shared" si="8"/>
         <v>22</v>
       </c>
@@ -4119,13 +4263,13 @@
         <f t="shared" si="9"/>
         <v>00010110</v>
       </c>
-      <c r="D37" s="38" t="str">
+      <c r="D37" s="22" t="str">
         <f t="shared" si="10"/>
         <v>01011000</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="57">
+      <c r="A38">
         <f t="shared" si="8"/>
         <v>48</v>
       </c>
@@ -4136,9 +4280,130 @@
         <f t="shared" si="9"/>
         <v>00110000</v>
       </c>
-      <c r="D38" s="38" t="str">
+      <c r="D38" s="22" t="str">
         <f t="shared" si="10"/>
         <v>00011100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C83CE775-DCD6-49CA-AB52-2CD16E8062AA}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="95"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="95"/>
+      <c r="D2" t="s">
+        <v>338</v>
+      </c>
+      <c r="E2" s="58">
+        <v>4294967295</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>331</v>
+      </c>
+      <c r="C4" t="s">
+        <v>339</v>
+      </c>
+      <c r="D4" t="s">
+        <v>340</v>
+      </c>
+      <c r="E4" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>332</v>
+      </c>
+      <c r="B5" s="58">
+        <v>1476099196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>333</v>
+      </c>
+      <c r="B6" s="58">
+        <v>12543665</v>
+      </c>
+      <c r="C6" s="62">
+        <f>E2-B5+B6</f>
+        <v>2831411764</v>
+      </c>
+      <c r="D6" s="96">
+        <f>C6/1000000</f>
+        <v>2831.4117639999999</v>
+      </c>
+      <c r="E6" s="96">
+        <f>D6/60</f>
+        <v>47.190196066666665</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>334</v>
+      </c>
+      <c r="B7" s="58">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>335</v>
+      </c>
+      <c r="B8" s="58">
+        <v>2818868100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>337</v>
+      </c>
+      <c r="B9" s="58">
+        <v>12518695</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>264</v>
+      </c>
+      <c r="B10" s="58">
+        <v>9045</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>336</v>
+      </c>
+      <c r="B11" s="58">
+        <v>1384</v>
+      </c>
+      <c r="D11" s="87">
+        <f>B9/B10</f>
+        <v>1384.0458817025981</v>
       </c>
     </row>
   </sheetData>
@@ -4167,7 +4432,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="74" t="s">
         <v>230</v>
       </c>
       <c r="B1" t="s">
@@ -4290,10 +4555,10 @@
       <c r="J4" t="s">
         <v>265</v>
       </c>
-      <c r="K4" s="65">
+      <c r="K4" s="58">
         <v>36965</v>
       </c>
-      <c r="L4" s="65">
+      <c r="L4" s="58">
         <v>43897</v>
       </c>
       <c r="M4">
@@ -4308,7 +4573,7 @@
       <c r="P4">
         <v>20856</v>
       </c>
-      <c r="Q4" s="65">
+      <c r="Q4" s="58">
         <v>43919</v>
       </c>
       <c r="R4">
@@ -4340,10 +4605,10 @@
       <c r="J5" t="s">
         <v>266</v>
       </c>
-      <c r="K5" s="65">
+      <c r="K5" s="58">
         <v>89737</v>
       </c>
-      <c r="L5" s="65">
+      <c r="L5" s="58">
         <v>58716</v>
       </c>
       <c r="M5">
@@ -4358,7 +4623,7 @@
       <c r="P5">
         <v>113991</v>
       </c>
-      <c r="Q5" s="65">
+      <c r="Q5" s="58">
         <v>58739</v>
       </c>
       <c r="R5">
@@ -4387,59 +4652,59 @@
       <c r="J6" t="s">
         <v>269</v>
       </c>
-      <c r="K6" s="65">
+      <c r="K6" s="58">
         <f t="shared" ref="K6:U6" si="0">K5-K4</f>
         <v>52772</v>
       </c>
-      <c r="L6" s="65">
+      <c r="L6" s="58">
         <f t="shared" si="0"/>
         <v>14819</v>
       </c>
-      <c r="M6" s="65">
+      <c r="M6" s="58">
         <f t="shared" si="0"/>
         <v>151988</v>
       </c>
-      <c r="N6" s="65">
+      <c r="N6" s="58">
         <f t="shared" si="0"/>
         <v>151599</v>
       </c>
-      <c r="O6" s="65">
+      <c r="O6" s="58">
         <f t="shared" si="0"/>
         <v>168236</v>
       </c>
-      <c r="P6" s="65">
+      <c r="P6" s="58">
         <f t="shared" si="0"/>
         <v>93135</v>
       </c>
-      <c r="Q6" s="65">
+      <c r="Q6" s="58">
         <f t="shared" si="0"/>
         <v>14820</v>
       </c>
-      <c r="R6" s="65">
+      <c r="R6" s="58">
         <f t="shared" si="0"/>
         <v>76522</v>
       </c>
-      <c r="S6" s="65">
+      <c r="S6" s="58">
         <f t="shared" si="0"/>
         <v>58032</v>
       </c>
-      <c r="T6" s="65">
+      <c r="T6" s="58">
         <f t="shared" si="0"/>
         <v>60002</v>
       </c>
-      <c r="U6" s="65">
+      <c r="U6" s="58">
         <f t="shared" si="0"/>
         <v>58031</v>
       </c>
-      <c r="V6" s="65">
+      <c r="V6" s="58">
         <f t="shared" ref="V6:W6" si="1">V5-V4</f>
         <v>3049994</v>
       </c>
-      <c r="W6" s="65">
+      <c r="W6" s="58">
         <f t="shared" si="1"/>
         <v>8461219</v>
       </c>
-      <c r="X6" s="65">
+      <c r="X6" s="58">
         <f t="shared" ref="X6" si="2">X5-X4</f>
         <v>77989</v>
       </c>
@@ -4460,81 +4725,81 @@
       <c r="J7" t="s">
         <v>267</v>
       </c>
-      <c r="K7" s="87">
+      <c r="K7" s="76">
         <f t="shared" ref="K7:U7" si="3">(K6*0.000001)/K3</f>
         <v>1.7828378378378378E-4</v>
       </c>
-      <c r="L7" s="87">
+      <c r="L7" s="76">
         <f t="shared" si="3"/>
         <v>3.7047499999999997E-3</v>
       </c>
-      <c r="M7" s="87">
+      <c r="M7" s="76">
         <f t="shared" si="3"/>
         <v>1.4900784313725489E-3</v>
       </c>
-      <c r="N7" s="87">
+      <c r="N7" s="76">
         <f t="shared" si="3"/>
         <v>2.9153653846153843E-3</v>
       </c>
-      <c r="O7" s="87">
+      <c r="O7" s="76">
         <f t="shared" si="3"/>
         <v>3.2353076923076923E-3</v>
       </c>
-      <c r="P7" s="87">
+      <c r="P7" s="76">
         <f t="shared" si="3"/>
         <v>3.1464527027027026E-4</v>
       </c>
-      <c r="Q7" s="87">
+      <c r="Q7" s="76">
         <f t="shared" si="3"/>
         <v>3.705E-3</v>
       </c>
-      <c r="R7" s="87">
+      <c r="R7" s="76">
         <f t="shared" si="3"/>
         <v>2.5852027027027023E-4</v>
       </c>
-      <c r="S7" s="87">
+      <c r="S7" s="76">
         <f t="shared" si="3"/>
         <v>1.9605405405405404E-4</v>
       </c>
-      <c r="T7" s="87">
+      <c r="T7" s="76">
         <f t="shared" si="3"/>
         <v>2.0339661016949151E-4</v>
       </c>
-      <c r="U7" s="87">
+      <c r="U7" s="76">
         <f t="shared" si="3"/>
         <v>1.9671525423728813E-4</v>
       </c>
-      <c r="V7" s="87">
+      <c r="V7" s="76">
         <f t="shared" ref="V7:W7" si="4">(V6*0.000001)/V3</f>
         <v>8.1879033557046975E-4</v>
       </c>
-      <c r="W7" s="87">
+      <c r="W7" s="76">
         <f t="shared" si="4"/>
         <v>8.1553918072289151E-4</v>
       </c>
-      <c r="X7" s="87">
+      <c r="X7" s="76">
         <f t="shared" ref="X7:Z7" si="5">(X6*0.000001)/X3</f>
         <v>2.2030790960451979E-4</v>
       </c>
-      <c r="Y7" s="87">
+      <c r="Y7" s="76">
         <f t="shared" si="5"/>
         <v>1.4106126036484245E-3</v>
       </c>
-      <c r="Z7" s="87">
+      <c r="Z7" s="76">
         <f t="shared" si="5"/>
         <v>1.1817542288557214E-3</v>
       </c>
-      <c r="AA7" s="87">
+      <c r="AA7" s="76">
         <f t="shared" ref="AA7:AB7" si="6">(AA6*0.000001)/AA3</f>
         <v>1.178326368159204E-3</v>
       </c>
-      <c r="AB7" s="87">
+      <c r="AB7" s="76">
         <f t="shared" si="6"/>
         <v>1.1413300165837479E-3</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A8" s="85" t="s">
+      <c r="A8" s="74" t="s">
         <v>231</v>
       </c>
       <c r="B8" t="s">
@@ -4543,75 +4808,75 @@
       <c r="J8" t="s">
         <v>268</v>
       </c>
-      <c r="K8" s="65">
+      <c r="K8" s="58">
         <f t="shared" ref="K8:U8" si="7">(1/K7)</f>
         <v>5609.0350943682261</v>
       </c>
-      <c r="L8" s="65">
+      <c r="L8" s="58">
         <f t="shared" si="7"/>
         <v>269.92374654160204</v>
       </c>
-      <c r="M8" s="65">
+      <c r="M8" s="58">
         <f t="shared" si="7"/>
         <v>671.10561360107386</v>
       </c>
-      <c r="N8" s="65">
+      <c r="N8" s="58">
         <f t="shared" si="7"/>
         <v>343.01017816740222</v>
       </c>
-      <c r="O8" s="65">
+      <c r="O8" s="58">
         <f t="shared" si="7"/>
         <v>309.08961221141732</v>
       </c>
-      <c r="P8" s="65">
+      <c r="P8" s="58">
         <f t="shared" si="7"/>
         <v>3178.1822086218931</v>
       </c>
-      <c r="Q8" s="65">
+      <c r="Q8" s="58">
         <f t="shared" si="7"/>
         <v>269.90553306342781</v>
       </c>
-      <c r="R8" s="65">
+      <c r="R8" s="58">
         <f t="shared" si="7"/>
         <v>3868.168631243303</v>
       </c>
-      <c r="S8" s="65">
+      <c r="S8" s="58">
         <f t="shared" si="7"/>
         <v>5100.6341328921981</v>
       </c>
-      <c r="T8" s="65">
+      <c r="T8" s="58">
         <f t="shared" si="7"/>
         <v>4916.5027832405585</v>
       </c>
-      <c r="U8" s="65">
+      <c r="U8" s="58">
         <f t="shared" si="7"/>
         <v>5083.4898588685364</v>
       </c>
-      <c r="V8" s="65">
+      <c r="V8" s="58">
         <f t="shared" ref="V8:W8" si="8">(1/V7)</f>
         <v>1221.3138779945141</v>
       </c>
-      <c r="W8" s="65">
+      <c r="W8" s="58">
         <f t="shared" si="8"/>
         <v>1226.1826576052458</v>
       </c>
-      <c r="X8" s="65">
+      <c r="X8" s="58">
         <f t="shared" ref="X8:Z8" si="9">(1/X7)</f>
         <v>4539.1016681839747</v>
       </c>
-      <c r="Y8" s="65">
+      <c r="Y8" s="58">
         <f t="shared" si="9"/>
         <v>708.91185674478493</v>
       </c>
-      <c r="Z8" s="65">
+      <c r="Z8" s="58">
         <f t="shared" si="9"/>
         <v>846.19963743923995</v>
       </c>
-      <c r="AA8" s="65">
+      <c r="AA8" s="58">
         <f t="shared" ref="AA8:AB8" si="10">(1/AA7)</f>
         <v>848.66131067083927</v>
       </c>
-      <c r="AB8" s="65">
+      <c r="AB8" s="58">
         <f t="shared" si="10"/>
         <v>876.17077047813063</v>
       </c>
@@ -4644,10 +4909,10 @@
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="M13" s="65"/>
+      <c r="M13" s="58"/>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="M14" s="65"/>
+      <c r="M14" s="58"/>
       <c r="X14">
         <v>1</v>
       </c>
@@ -4664,7 +4929,7 @@
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A16" s="85" t="s">
+      <c r="A16" s="74" t="s">
         <v>242</v>
       </c>
       <c r="B16" t="s">
@@ -4702,7 +4967,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="85" t="s">
+      <c r="A24" s="74" t="s">
         <v>243</v>
       </c>
       <c r="B24" t="s">
@@ -4745,7 +5010,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="85" t="s">
+      <c r="A33" s="74" t="s">
         <v>248</v>
       </c>
       <c r="B33" t="s">
@@ -4758,7 +5023,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="85" t="s">
+      <c r="A36" s="74" t="s">
         <v>281</v>
       </c>
     </row>
@@ -4773,7 +5038,7 @@
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="85" t="s">
+      <c r="A40" s="74" t="s">
         <v>284</v>
       </c>
     </row>
@@ -4793,7 +5058,7 @@
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="85" t="s">
+      <c r="A44" s="74" t="s">
         <v>291</v>
       </c>
     </row>
@@ -4818,7 +5083,7 @@
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="85" t="s">
+      <c r="A50" s="74" t="s">
         <v>271</v>
       </c>
     </row>
@@ -4843,7 +5108,7 @@
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="85" t="s">
+      <c r="A56" s="74" t="s">
         <v>272</v>
       </c>
     </row>
@@ -4879,183 +5144,183 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.28515625" style="89" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" style="90" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="90" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="90" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="90" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="90" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" style="90" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="90"/>
-    <col min="9" max="9" width="9.140625" style="89"/>
+    <col min="1" max="1" width="31.28515625" style="78" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" style="79" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="79" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="79" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="79" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" style="79" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" style="79" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="79"/>
+    <col min="9" max="9" width="9.140625" style="78"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="90" t="s">
+      <c r="B1" s="79" t="s">
         <v>292</v>
       </c>
-      <c r="C1" s="91" t="s">
+      <c r="C1" s="80" t="s">
         <v>293</v>
       </c>
-      <c r="D1" s="90" t="s">
+      <c r="D1" s="79" t="s">
         <v>294</v>
       </c>
-      <c r="E1" s="90" t="s">
+      <c r="E1" s="79" t="s">
         <v>295</v>
       </c>
-      <c r="F1" s="90" t="s">
+      <c r="F1" s="79" t="s">
         <v>296</v>
       </c>
-      <c r="G1" s="90" t="s">
+      <c r="G1" s="79" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="81" t="s">
         <v>230</v>
       </c>
-      <c r="B2" s="91"/>
+      <c r="B2" s="80"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="79" t="s">
         <v>232</v>
       </c>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="79" t="s">
         <v>298</v>
       </c>
-      <c r="C3" s="90" t="s">
+      <c r="C3" s="79" t="s">
         <v>298</v>
       </c>
-      <c r="D3" s="90">
+      <c r="D3" s="79">
         <v>0</v>
       </c>
-      <c r="E3" s="90">
+      <c r="E3" s="79">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="92" t="s">
+      <c r="A5" s="81" t="s">
         <v>231</v>
       </c>
-      <c r="B5" s="91"/>
+      <c r="B5" s="80"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="90" t="s">
+      <c r="A6" s="79" t="s">
         <v>235</v>
       </c>
-      <c r="B6" s="90" t="s">
+      <c r="B6" s="79" t="s">
         <v>299</v>
       </c>
-      <c r="F6" s="90" t="s">
+      <c r="F6" s="79" t="s">
         <v>300</v>
       </c>
-      <c r="G6" s="90" t="s">
+      <c r="G6" s="79" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="92" t="s">
+      <c r="A8" s="81" t="s">
         <v>242</v>
       </c>
       <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="90" t="s">
+      <c r="A9" s="79" t="s">
         <v>241</v>
       </c>
-      <c r="B9" s="90" t="s">
+      <c r="B9" s="79" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="93" t="s">
+      <c r="A10" s="82" t="s">
         <v>302</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="93" t="s">
+      <c r="A11" s="82" t="s">
         <v>238</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="93" t="s">
+      <c r="A12" s="82" t="s">
         <v>239</v>
       </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="93" t="s">
+      <c r="A13" s="82" t="s">
         <v>240</v>
       </c>
       <c r="B13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="90" t="s">
+      <c r="B14" s="79" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="92" t="s">
+      <c r="A16" s="81" t="s">
         <v>243</v>
       </c>
       <c r="B16" s="1"/>
-      <c r="G16" s="90" t="s">
+      <c r="G16" s="79" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="24" x14ac:dyDescent="0.25">
-      <c r="A17" s="94" t="s">
+      <c r="A17" s="83" t="s">
         <v>304</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="G17" s="90" t="s">
+      <c r="G17" s="79" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="90" t="s">
+      <c r="B18" s="79" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="90" t="s">
+      <c r="A19" s="79" t="s">
         <v>245</v>
       </c>
       <c r="B19" s="1"/>
-      <c r="G19" s="90" t="s">
+      <c r="G19" s="79" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="90" t="s">
+      <c r="A20" s="79" t="s">
         <v>307</v>
       </c>
-      <c r="B20" s="90" t="s">
+      <c r="B20" s="79" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="92" t="s">
+      <c r="A22" s="81" t="s">
         <v>248</v>
       </c>
       <c r="B22" s="1"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="90" t="s">
+      <c r="A23" s="79" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="92" t="s">
+      <c r="A25" s="81" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="90" t="s">
+      <c r="A26" s="79" t="s">
         <v>282</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -5066,98 +5331,98 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="90" t="s">
+      <c r="A27" s="79" t="s">
         <v>311</v>
       </c>
       <c r="B27" s="1"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="92" t="s">
+      <c r="A29" s="81" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="89" t="s">
+      <c r="A30" s="78" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="89" t="s">
+      <c r="A31" s="78" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="89" t="s">
+      <c r="A32" s="78" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="92" t="s">
+      <c r="A33" s="81" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="89" t="s">
+      <c r="A34" s="78" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="89" t="s">
+      <c r="A35" s="78" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="89" t="s">
+      <c r="A36" s="78" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="89" t="s">
+      <c r="A37" s="78" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="92" t="s">
+      <c r="A39" s="81" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="89" t="s">
+      <c r="A40" s="78" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="89" t="s">
+      <c r="A41" s="78" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="89" t="s">
+      <c r="A42" s="78" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="89" t="s">
+      <c r="A43" s="78" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="92" t="s">
+      <c r="A45" s="81" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="89" t="s">
+      <c r="A46" s="78" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="89" t="s">
+      <c r="A47" s="78" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="89" t="s">
+      <c r="A48" s="78" t="s">
         <v>280</v>
       </c>
     </row>
@@ -5719,15 +5984,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="74" t="s">
         <v>261</v>
       </c>
-      <c r="B1" s="85" t="s">
+      <c r="B1" s="74" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="86">
+      <c r="A2" s="75">
         <v>14</v>
       </c>
       <c r="B2" t="s">
@@ -5735,10 +6000,10 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="86"/>
+      <c r="A3" s="75"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="86">
+      <c r="A4" s="75">
         <v>8</v>
       </c>
       <c r="B4" t="s">
@@ -5752,9 +6017,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8351D32F-052C-49B4-91CF-60F5FD05FC35}">
-  <dimension ref="A2:Z49"/>
+  <dimension ref="A2:Z50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A27" workbookViewId="0">
       <selection activeCell="O8" sqref="O8:S14"/>
     </sheetView>
   </sheetViews>
@@ -5766,7 +6031,8 @@
     <col min="5" max="5" width="10.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="1" customWidth="1"/>
     <col min="7" max="9" width="6" style="1" customWidth="1"/>
-    <col min="10" max="12" width="5.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.85546875" style="1" customWidth="1"/>
+    <col min="11" max="12" width="5.5703125" style="1" customWidth="1"/>
     <col min="13" max="14" width="6.140625" style="1" customWidth="1"/>
     <col min="15" max="15" width="20.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" style="19" customWidth="1"/>
@@ -5890,16 +6156,16 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="F6" s="2"/>
-      <c r="G6" s="98">
+      <c r="G6" s="91">
         <v>1</v>
       </c>
-      <c r="H6" s="99"/>
-      <c r="I6" s="99"/>
-      <c r="J6" s="98">
+      <c r="H6" s="92"/>
+      <c r="I6" s="92"/>
+      <c r="J6" s="91">
         <v>0</v>
       </c>
-      <c r="K6" s="99"/>
-      <c r="L6" s="99"/>
+      <c r="K6" s="92"/>
+      <c r="L6" s="92"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="X6" s="2" t="s">
@@ -5910,16 +6176,16 @@
       <c r="F7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="100" t="s">
+      <c r="G7" s="93" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="101"/>
-      <c r="I7" s="101"/>
-      <c r="J7" s="100" t="s">
+      <c r="H7" s="94"/>
+      <c r="I7" s="94"/>
+      <c r="J7" s="93" t="s">
         <v>38</v>
       </c>
-      <c r="K7" s="101"/>
-      <c r="L7" s="101"/>
+      <c r="K7" s="94"/>
+      <c r="L7" s="94"/>
       <c r="X7" s="1" t="s">
         <v>66</v>
       </c>
@@ -5934,21 +6200,21 @@
       <c r="F8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="100" t="s">
+      <c r="G8" s="93" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="101"/>
-      <c r="I8" s="101"/>
-      <c r="J8" s="100" t="s">
+      <c r="H8" s="94"/>
+      <c r="I8" s="94"/>
+      <c r="J8" s="93" t="s">
         <v>41</v>
       </c>
-      <c r="K8" s="101"/>
-      <c r="L8" s="101"/>
+      <c r="K8" s="94"/>
+      <c r="L8" s="94"/>
       <c r="O8" s="17"/>
-      <c r="P8" s="95" t="s">
+      <c r="P8" s="88" t="s">
         <v>59</v>
       </c>
-      <c r="Q8" s="96"/>
+      <c r="Q8" s="89"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
       <c r="Y8" s="1" t="s">
@@ -5962,27 +6228,27 @@
       <c r="F9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="100" t="s">
+      <c r="G9" s="93" t="s">
         <v>56</v>
       </c>
-      <c r="H9" s="101"/>
-      <c r="I9" s="101"/>
-      <c r="J9" s="100" t="s">
+      <c r="H9" s="94"/>
+      <c r="I9" s="94"/>
+      <c r="J9" s="93" t="s">
         <v>57</v>
       </c>
-      <c r="K9" s="101"/>
-      <c r="L9" s="101"/>
-      <c r="O9" s="58" t="s">
+      <c r="K9" s="94"/>
+      <c r="L9" s="94"/>
+      <c r="O9" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="P9" s="59">
+      <c r="P9" s="53">
         <v>1</v>
       </c>
-      <c r="Q9" s="59">
+      <c r="Q9" s="53">
         <v>0</v>
       </c>
-      <c r="R9" s="41"/>
-      <c r="S9" s="54" t="s">
+      <c r="R9" s="38"/>
+      <c r="S9" s="49" t="s">
         <v>144</v>
       </c>
       <c r="X9" s="1" t="s">
@@ -5999,27 +6265,27 @@
       <c r="F10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="100" t="s">
+      <c r="G10" s="93" t="s">
         <v>81</v>
       </c>
-      <c r="H10" s="101"/>
-      <c r="I10" s="101"/>
-      <c r="J10" s="100" t="s">
+      <c r="H10" s="94"/>
+      <c r="I10" s="94"/>
+      <c r="J10" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="K10" s="101"/>
-      <c r="L10" s="101"/>
-      <c r="O10" s="42" t="s">
+      <c r="K10" s="94"/>
+      <c r="L10" s="94"/>
+      <c r="O10" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="P10" s="43">
+      <c r="P10" s="19">
         <v>0</v>
       </c>
-      <c r="Q10" s="43">
+      <c r="Q10" s="19">
         <v>0</v>
       </c>
-      <c r="R10" s="44"/>
-      <c r="S10" s="45">
+      <c r="R10" s="1"/>
+      <c r="S10" s="40">
         <v>0</v>
       </c>
       <c r="Y10" s="1" t="s">
@@ -6030,17 +6296,17 @@
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="O11" s="46" t="s">
+      <c r="O11" s="41" t="s">
         <v>148</v>
       </c>
-      <c r="P11" s="43">
+      <c r="P11" s="19">
         <v>0</v>
       </c>
-      <c r="Q11" s="43">
+      <c r="Q11" s="19">
         <v>1</v>
       </c>
-      <c r="R11" s="44"/>
-      <c r="S11" s="45">
+      <c r="R11" s="1"/>
+      <c r="S11" s="40">
         <v>1</v>
       </c>
       <c r="X11" s="1" t="s">
@@ -6058,21 +6324,21 @@
         <v>58</v>
       </c>
       <c r="E12" s="20"/>
-      <c r="O12" s="47" t="s">
+      <c r="O12" s="42" t="s">
         <v>149</v>
       </c>
-      <c r="P12" s="43">
+      <c r="P12" s="19">
         <v>1</v>
       </c>
-      <c r="Q12" s="43">
+      <c r="Q12" s="19">
         <v>0</v>
       </c>
-      <c r="R12" s="44"/>
-      <c r="S12" s="45">
+      <c r="R12" s="1"/>
+      <c r="S12" s="40">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="3" t="s">
         <v>54</v>
       </c>
@@ -6082,17 +6348,23 @@
       <c r="E13" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="O13" s="48" t="s">
+      <c r="I13" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="O13" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="P13" s="49">
+      <c r="P13" s="44">
         <v>1</v>
       </c>
-      <c r="Q13" s="49">
+      <c r="Q13" s="44">
         <v>1</v>
       </c>
-      <c r="R13" s="50"/>
-      <c r="S13" s="51">
+      <c r="R13" s="45"/>
+      <c r="S13" s="46">
         <v>3</v>
       </c>
     </row>
@@ -6100,7 +6372,7 @@
       <c r="C14" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="E14" s="52">
+      <c r="E14" s="47">
         <v>0</v>
       </c>
       <c r="O14" s="17"/>
@@ -6112,335 +6384,333 @@
       <c r="D15" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E15" s="52">
+      <c r="E15" s="47">
         <v>2</v>
       </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0</v>
+      </c>
       <c r="O15" s="18"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C16" s="4" t="s">
+      <c r="D16" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="47">
+        <v>3</v>
+      </c>
+      <c r="I16" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="J16" s="84">
+        <f>I16/0.125</f>
+        <v>188</v>
+      </c>
+      <c r="O16" s="18"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C17" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="53">
+      <c r="D17" s="1"/>
+      <c r="E17" s="48">
         <v>2</v>
       </c>
-      <c r="O16" s="17"/>
-    </row>
-    <row r="17" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="C17" s="4" t="s">
+      <c r="I17" s="1">
+        <v>24.7</v>
+      </c>
+      <c r="J17" s="84">
+        <f>I17/0.125</f>
+        <v>197.6</v>
+      </c>
+      <c r="O17" s="17"/>
+    </row>
+    <row r="18" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="C18" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E17" s="52"/>
-      <c r="O17" s="2" t="s">
+      <c r="E18" s="47"/>
+      <c r="I18" s="1">
+        <v>116.25</v>
+      </c>
+      <c r="O18" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="P17" s="16" t="s">
+      <c r="P18" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="Q17" s="16" t="s">
+      <c r="Q18" s="16" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D18" s="4" t="s">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D19" s="1"/>
+      <c r="N19" s="1">
+        <v>0</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P19" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q19" s="16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="D20" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E20" s="47">
+        <v>2</v>
+      </c>
+      <c r="N20" s="1">
+        <v>1</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="P20" s="19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="D21" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47">
+        <v>1</v>
+      </c>
+      <c r="G21" s="47">
+        <v>2</v>
+      </c>
+      <c r="N21" s="1">
+        <v>2</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="P21" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>1</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="E22" s="47"/>
+      <c r="N22" s="1">
+        <v>3</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="P22" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D23" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="52">
+      <c r="E23" s="47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C24" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E24" s="47"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D25" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="47">
         <v>3</v>
       </c>
-      <c r="N18" s="1">
+    </row>
+    <row r="26" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="C26" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E26" s="47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C27" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E27" s="47"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D28" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="47">
         <v>0</v>
       </c>
-      <c r="O18" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="P18" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q18" s="16" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="D19" s="4" t="s">
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E29" s="47"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
+        <v>1</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="E30" s="47"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C31" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E31" s="47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D32" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E32" s="47"/>
+    </row>
+    <row r="33" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="D33" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E33" s="47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="3:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="C34" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="E19" s="52">
+      <c r="E34" s="47">
         <v>2</v>
       </c>
-      <c r="N19" s="1">
-        <v>1</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="P19" s="19" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" ht="45" x14ac:dyDescent="0.25">
-      <c r="D20" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="E20" s="52"/>
-      <c r="F20" s="52">
-        <v>1</v>
-      </c>
-      <c r="G20" s="52">
-        <v>2</v>
-      </c>
-      <c r="N20" s="1">
-        <v>2</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="P20" s="19">
+    </row>
+    <row r="35" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C35" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E35" s="47"/>
+    </row>
+    <row r="36" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="D36" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E36" s="47">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
-        <v>1</v>
-      </c>
-      <c r="B21" s="40" t="s">
-        <v>156</v>
-      </c>
-      <c r="E21" s="52"/>
-      <c r="N21" s="1">
-        <v>3</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="P21" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D22" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E22" s="52">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C23" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E23" s="52"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D24" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E24" s="52">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="C25" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="E25" s="52">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C26" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="E26" s="52"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D27" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E27" s="52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E28" s="52"/>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="6">
-        <v>1</v>
-      </c>
-      <c r="B29" s="40" t="s">
-        <v>159</v>
-      </c>
-      <c r="E29" s="52"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C30" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E30" s="52">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D31" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E31" s="52"/>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D32" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E32" s="52">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="3:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="C33" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="E33" s="52">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C34" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="E34" s="52"/>
-    </row>
-    <row r="35" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="D35" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E35" s="52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="E36" s="52"/>
-    </row>
     <row r="37" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C37" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E37" s="52"/>
+      <c r="E37" s="47"/>
     </row>
     <row r="38" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C38" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E38" s="47"/>
+    </row>
+    <row r="39" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C39" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="E38" s="52"/>
-    </row>
-    <row r="39" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C39" s="1"/>
-      <c r="E39" s="52"/>
+      <c r="E39" s="47"/>
     </row>
     <row r="40" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="1"/>
+      <c r="E40" s="47"/>
+    </row>
+    <row r="41" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C41" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3" t="s">
+      <c r="D41" s="3"/>
+      <c r="E41" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="F40" s="60" t="s">
+      <c r="F41" s="54" t="s">
         <v>191</v>
       </c>
-      <c r="G40" s="2" t="s">
+      <c r="G41" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="H41" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="I40" s="2" t="s">
+      <c r="I41" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="J40" s="2" t="s">
+      <c r="J41" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="K40" s="2"/>
-      <c r="T40" s="2" t="s">
+      <c r="K41" s="2"/>
+      <c r="T41" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="U40" s="1" t="s">
+      <c r="U41" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C41" s="1" t="s">
+    <row r="42" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C42" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="E41" s="52">
+      <c r="E42" s="47">
         <v>3</v>
       </c>
-      <c r="F41" s="6">
+      <c r="F42" s="6">
         <v>1</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="G42" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="J41" s="1" t="s">
+      <c r="J42" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="T41" s="2" t="s">
+      <c r="T42" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="U41" s="1" t="s">
+      <c r="U42" s="1" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="42" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C42" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="E42" s="52">
-        <v>8</v>
-      </c>
-      <c r="F42" s="6">
-        <v>4</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="J42" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="T42" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="U42" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="43" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C43" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="E43" s="52">
-        <v>10</v>
+        <v>172</v>
+      </c>
+      <c r="E43" s="47">
+        <v>8</v>
       </c>
       <c r="F43" s="6">
         <v>4</v>
@@ -6455,18 +6725,24 @@
         <v>182</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
+      </c>
+      <c r="T43" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="U43" s="1" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="44" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C44" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="E44" s="1">
-        <v>11</v>
+        <v>173</v>
+      </c>
+      <c r="E44" s="47">
+        <v>10</v>
       </c>
       <c r="F44" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>180</v>
@@ -6474,12 +6750,32 @@
       <c r="H44" s="1" t="s">
         <v>181</v>
       </c>
+      <c r="I44" s="1" t="s">
+        <v>182</v>
+      </c>
       <c r="J44" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="45" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C45" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="E45" s="1">
+        <v>11</v>
+      </c>
+      <c r="F45" s="6">
+        <v>3</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="J45" s="1" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="45" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="F45" s="6"/>
     </row>
     <row r="46" spans="3:21" x14ac:dyDescent="0.25">
       <c r="F46" s="6"/>
@@ -6488,22 +6784,25 @@
       <c r="F47" s="6"/>
     </row>
     <row r="48" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C48" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="E48" s="1">
-        <v>20</v>
-      </c>
       <c r="F48" s="6"/>
     </row>
     <row r="49" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C49" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="E49" s="1">
+        <v>20</v>
+      </c>
+      <c r="F49" s="6"/>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C50" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="E49" s="1">
+      <c r="E50" s="1">
         <v>21</v>
       </c>
-      <c r="F49" s="6"/>
+      <c r="F50" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -6529,6 +6828,398 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FABCE0B6-7AF3-4998-B1DC-5B32CFF531D9}">
+  <dimension ref="A1:Q30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="27.140625" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
+    <col min="14" max="14" width="21.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="6"/>
+      <c r="B1" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:17" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="47">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="88" t="s">
+        <v>59</v>
+      </c>
+      <c r="P3" s="89"/>
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E4" s="47">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="85">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="N4" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="O4" s="53">
+        <v>1</v>
+      </c>
+      <c r="P4" s="53">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="49" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="E5" s="47">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="85">
+        <v>23.5</v>
+      </c>
+      <c r="J5" s="84">
+        <f>I5/0.125</f>
+        <v>188</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="N5" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="O5" s="19">
+        <v>0</v>
+      </c>
+      <c r="P5" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="48">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="85">
+        <v>24.7</v>
+      </c>
+      <c r="J6" s="84">
+        <f>I6/0.125</f>
+        <v>197.6</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="N6" s="41" t="s">
+        <v>148</v>
+      </c>
+      <c r="O6" s="19">
+        <v>0</v>
+      </c>
+      <c r="P6" s="19">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="I7" s="85">
+        <v>116.25</v>
+      </c>
+      <c r="J7" s="84">
+        <f t="shared" ref="J7:J11" si="0">I7/0.125</f>
+        <v>930</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="N7" s="42" t="s">
+        <v>149</v>
+      </c>
+      <c r="O7" s="19">
+        <v>1</v>
+      </c>
+      <c r="P7" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="D8" t="s">
+        <v>326</v>
+      </c>
+      <c r="E8" s="47">
+        <v>3</v>
+      </c>
+      <c r="I8" s="85">
+        <v>119.25</v>
+      </c>
+      <c r="J8" s="84">
+        <f t="shared" si="0"/>
+        <v>954</v>
+      </c>
+      <c r="K8" s="1"/>
+      <c r="N8" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="O8" s="44">
+        <v>1</v>
+      </c>
+      <c r="P8" s="44">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="D9" t="s">
+        <v>327</v>
+      </c>
+      <c r="I9" s="86">
+        <v>119.8</v>
+      </c>
+      <c r="J9" s="84">
+        <f t="shared" si="0"/>
+        <v>958.4</v>
+      </c>
+      <c r="K9" s="1"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="D10" t="s">
+        <v>328</v>
+      </c>
+      <c r="I10" s="86">
+        <v>121.35</v>
+      </c>
+      <c r="J10" s="84">
+        <f t="shared" si="0"/>
+        <v>970.8</v>
+      </c>
+      <c r="K10" s="1"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="D11" t="s">
+        <v>326</v>
+      </c>
+      <c r="E11" s="47">
+        <v>2</v>
+      </c>
+      <c r="I11" s="85">
+        <v>121.7</v>
+      </c>
+      <c r="J11" s="84">
+        <f t="shared" si="0"/>
+        <v>973.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C13" s="4"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C14" s="4"/>
+      <c r="D14" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="85">
+        <f>I5-I4</f>
+        <v>23.5</v>
+      </c>
+      <c r="J14" s="84">
+        <f>I14/0.125</f>
+        <v>188</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C15" s="4"/>
+      <c r="D15" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="E15" s="47"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="86">
+        <f>I11-I8</f>
+        <v>2.4500000000000028</v>
+      </c>
+      <c r="J15" s="84">
+        <f>I15/0.125</f>
+        <v>19.600000000000023</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="85"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I17" s="86"/>
+    </row>
+    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I18" s="86"/>
+    </row>
+    <row r="19" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I19" s="86"/>
+    </row>
+    <row r="20" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I20" s="86"/>
+    </row>
+    <row r="21" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I21" s="86"/>
+    </row>
+    <row r="22" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I22" s="86"/>
+    </row>
+    <row r="23" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I23" s="87"/>
+    </row>
+    <row r="24" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I24" s="87"/>
+    </row>
+    <row r="25" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I25" s="87"/>
+    </row>
+    <row r="26" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I26" s="87"/>
+    </row>
+    <row r="27" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I27" s="87"/>
+    </row>
+    <row r="28" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I28" s="87"/>
+    </row>
+    <row r="29" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I29" s="87"/>
+    </row>
+    <row r="30" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I30" s="87"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="O3:P3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E8953BE-283E-447B-901F-738677242859}">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -6631,7 +7322,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{501AD065-09D6-4E30-BC30-53C37491F725}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -6760,100 +7451,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3524476A-77A4-4787-9A72-750F9A8F2315}">
-  <dimension ref="A1:L10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.140625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="10"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2"/>
-      <c r="E2"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="11">
-        <f>1.25*(1+B5/B6)</f>
-        <v>3.125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="B5" s="10">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="B6" s="10">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="10">
-        <v>3.3</v>
-      </c>
-      <c r="L8"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="12">
-        <f>B8/(B5+B6)*1000000</f>
-        <v>3300</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="K10"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
xmodem with data transfer issues
</commit_message>
<xml_diff>
--- a/H89_ESP32 Commands.xlsx
+++ b/H89_ESP32 Commands.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dev\ESP32\H89_ESP32\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dev\ESP32\H89_ESP32_RTOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9924255D-46E4-4652-B7AE-BC2973E51010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D4D64F-F870-4042-81C8-57B7FA9F52C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="23865" windowHeight="11385" tabRatio="636" activeTab="6" xr2:uid="{D2F2CCC8-256C-4E0F-AF5D-63EDFF332B66}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11385" tabRatio="636" xr2:uid="{D2F2CCC8-256C-4E0F-AF5D-63EDFF332B66}"/>
   </bookViews>
   <sheets>
     <sheet name="Cmd Summary" sheetId="8" r:id="rId1"/>
@@ -1770,7 +1770,7 @@
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2026,19 +2026,18 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2536,8 +2535,8 @@
   </sheetPr>
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6289,16 +6288,16 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="F6" s="2"/>
-      <c r="G6" s="99">
+      <c r="G6" s="101">
         <v>1</v>
       </c>
-      <c r="H6" s="100"/>
-      <c r="I6" s="100"/>
-      <c r="J6" s="99">
+      <c r="H6" s="102"/>
+      <c r="I6" s="102"/>
+      <c r="J6" s="101">
         <v>0</v>
       </c>
-      <c r="K6" s="100"/>
-      <c r="L6" s="100"/>
+      <c r="K6" s="102"/>
+      <c r="L6" s="102"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="X6" s="2" t="s">
@@ -6309,16 +6308,16 @@
       <c r="F7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="101" t="s">
+      <c r="G7" s="99" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="102"/>
-      <c r="I7" s="102"/>
-      <c r="J7" s="101" t="s">
+      <c r="H7" s="100"/>
+      <c r="I7" s="100"/>
+      <c r="J7" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="K7" s="102"/>
-      <c r="L7" s="102"/>
+      <c r="K7" s="100"/>
+      <c r="L7" s="100"/>
       <c r="X7" s="1" t="s">
         <v>66</v>
       </c>
@@ -6333,16 +6332,16 @@
       <c r="F8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="101" t="s">
+      <c r="G8" s="99" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="102"/>
-      <c r="I8" s="102"/>
-      <c r="J8" s="101" t="s">
+      <c r="H8" s="100"/>
+      <c r="I8" s="100"/>
+      <c r="J8" s="99" t="s">
         <v>41</v>
       </c>
-      <c r="K8" s="102"/>
-      <c r="L8" s="102"/>
+      <c r="K8" s="100"/>
+      <c r="L8" s="100"/>
       <c r="O8" s="17"/>
       <c r="P8" s="96" t="s">
         <v>59</v>
@@ -6361,16 +6360,16 @@
       <c r="F9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="101" t="s">
+      <c r="G9" s="99" t="s">
         <v>56</v>
       </c>
-      <c r="H9" s="102"/>
-      <c r="I9" s="102"/>
-      <c r="J9" s="101" t="s">
+      <c r="H9" s="100"/>
+      <c r="I9" s="100"/>
+      <c r="J9" s="99" t="s">
         <v>57</v>
       </c>
-      <c r="K9" s="102"/>
-      <c r="L9" s="102"/>
+      <c r="K9" s="100"/>
+      <c r="L9" s="100"/>
       <c r="O9" s="52" t="s">
         <v>64</v>
       </c>
@@ -6398,16 +6397,16 @@
       <c r="F10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="101" t="s">
+      <c r="G10" s="99" t="s">
         <v>81</v>
       </c>
-      <c r="H10" s="102"/>
-      <c r="I10" s="102"/>
-      <c r="J10" s="101" t="s">
+      <c r="H10" s="100"/>
+      <c r="I10" s="100"/>
+      <c r="J10" s="99" t="s">
         <v>82</v>
       </c>
-      <c r="K10" s="102"/>
-      <c r="L10" s="102"/>
+      <c r="K10" s="100"/>
+      <c r="L10" s="100"/>
       <c r="O10" s="39" t="s">
         <v>60</v>
       </c>
@@ -6939,17 +6938,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="J8:L8"/>
     <mergeCell ref="P8:Q8"/>
     <mergeCell ref="J9:L9"/>
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="G9:I9"/>
     <mergeCell ref="G10:I10"/>
     <mergeCell ref="J10:L10"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="J8:L8"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6967,8 +6966,8 @@
   </sheetPr>
   <dimension ref="A1:S58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8029,7 +8028,7 @@
       </c>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B37" s="103" t="s">
+      <c r="B37" s="71" t="s">
         <v>369</v>
       </c>
       <c r="C37" s="71" t="s">
@@ -8115,7 +8114,7 @@
       </c>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B39" s="103" t="s">
+      <c r="B39" s="71" t="s">
         <v>369</v>
       </c>
       <c r="C39" s="71" t="s">

</xml_diff>